<commit_message>
add column overtime form
</commit_message>
<xml_diff>
--- a/overtime/static/OT_Request_Template.xlsx
+++ b/overtime/static/OT_Request_Template.xlsx
@@ -11,8 +11,9 @@
     <sheet name="Template" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Template!$A$1:$I$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Template!$A$1:$I$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Template!$A$1:$J$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Template!$A$1:$J$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Template!$A$1:$J$43</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -38,6 +39,7 @@
         <color rgb="FFFFFFFF"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">加     班     申     请     单
 </t>
@@ -63,6 +65,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">部门 </t>
     </r>
@@ -82,6 +85,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">工程部</t>
     </r>
@@ -103,6 +107,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">日期 </t>
     </r>
@@ -133,6 +138,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">项次
 </t>
@@ -155,6 +161,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">姓名
 </t>
@@ -177,6 +184,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">工號
 </t>
@@ -199,6 +207,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">预计加班时间
 </t>
@@ -222,6 +231,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">实际加班时间
 </t>
@@ -244,6 +254,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">实际加班时数
 </t>
@@ -260,12 +271,16 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Project Number</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">加 班 原 因
 </t>
@@ -288,6 +303,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> 填表
  </t>
@@ -310,6 +326,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主管
 </t>
@@ -332,6 +349,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">经理
 </t>
@@ -348,26 +366,8 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  总经理  
-  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">General Manager:      </t>
-    </r>
+    <t xml:space="preserve">  总经理  
+  General Manager:      </t>
   </si>
   <si>
     <r>
@@ -376,6 +376,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">人事
  </t>
@@ -408,6 +409,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">員工需經理</t>
     </r>
@@ -427,6 +429,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主管</t>
     </r>
@@ -446,6 +449,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">總經理簽名</t>
     </r>
@@ -465,6 +469,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">再交於人事部即可生效</t>
     </r>
@@ -502,6 +507,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主管需總經理簽名</t>
     </r>
@@ -521,6 +527,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">再交於人事部即可生效</t>
     </r>
@@ -601,12 +608,14 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -628,6 +637,7 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
@@ -641,12 +651,14 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -660,6 +672,7 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
@@ -673,6 +686,7 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -750,7 +764,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -843,14 +857,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -861,14 +867,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -920,14 +918,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -1084,21 +1075,22 @@
   <dimension ref="1:43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.57085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="2" width="3.8582995951417"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.35627530364372"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="2" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="2" width="12.6396761133603"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="2" width="9"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="9.25506072874494"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="12.1255060728745"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="4" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="11.6761133603239"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="2" width="9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1113,7 +1105,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
-      <c r="J1" s="0"/>
+      <c r="J1" s="5"/>
       <c r="K1" s="0"/>
       <c r="L1" s="0"/>
       <c r="M1" s="0"/>
@@ -2143,7 +2135,7 @@
         <v>2</v>
       </c>
       <c r="I2" s="7"/>
-      <c r="J2" s="0"/>
+      <c r="J2" s="7"/>
       <c r="K2" s="0"/>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
@@ -3171,6 +3163,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
     </row>
     <row r="4" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
@@ -3182,17 +3175,18 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10"/>
+      <c r="I4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="11"/>
+      <c r="K4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="L4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="M4" s="12" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3216,13 +3210,16 @@
       <c r="G5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="17"/>
-      <c r="J5" s="18"/>
+      <c r="I5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="17"/>
+      <c r="K5" s="18"/>
     </row>
-    <row r="6" s="24" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" s="19" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="20"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -3230,11 +3227,12 @@
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
-      <c r="H6" s="22"/>
+      <c r="H6" s="20"/>
       <c r="I6" s="22"/>
-      <c r="J6" s="23"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="18"/>
     </row>
-    <row r="7" s="24" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" s="19" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="20"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -3242,11 +3240,12 @@
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
-      <c r="H7" s="22"/>
+      <c r="H7" s="20"/>
       <c r="I7" s="22"/>
-      <c r="J7" s="23"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="18"/>
     </row>
-    <row r="8" s="24" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="20"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -3254,11 +3253,1025 @@
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
-      <c r="H8" s="21"/>
+      <c r="H8" s="20"/>
       <c r="I8" s="21"/>
-      <c r="J8" s="23"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0"/>
+      <c r="O8" s="0"/>
+      <c r="P8" s="0"/>
+      <c r="Q8" s="0"/>
+      <c r="R8" s="0"/>
+      <c r="S8" s="0"/>
+      <c r="T8" s="0"/>
+      <c r="U8" s="0"/>
+      <c r="V8" s="0"/>
+      <c r="W8" s="0"/>
+      <c r="X8" s="0"/>
+      <c r="Y8" s="0"/>
+      <c r="Z8" s="0"/>
+      <c r="AA8" s="0"/>
+      <c r="AB8" s="0"/>
+      <c r="AC8" s="0"/>
+      <c r="AD8" s="0"/>
+      <c r="AE8" s="0"/>
+      <c r="AF8" s="0"/>
+      <c r="AG8" s="0"/>
+      <c r="AH8" s="0"/>
+      <c r="AI8" s="0"/>
+      <c r="AJ8" s="0"/>
+      <c r="AK8" s="0"/>
+      <c r="AL8" s="0"/>
+      <c r="AM8" s="0"/>
+      <c r="AN8" s="0"/>
+      <c r="AO8" s="0"/>
+      <c r="AP8" s="0"/>
+      <c r="AQ8" s="0"/>
+      <c r="AR8" s="0"/>
+      <c r="AS8" s="0"/>
+      <c r="AT8" s="0"/>
+      <c r="AU8" s="0"/>
+      <c r="AV8" s="0"/>
+      <c r="AW8" s="0"/>
+      <c r="AX8" s="0"/>
+      <c r="AY8" s="0"/>
+      <c r="AZ8" s="0"/>
+      <c r="BA8" s="0"/>
+      <c r="BB8" s="0"/>
+      <c r="BC8" s="0"/>
+      <c r="BD8" s="0"/>
+      <c r="BE8" s="0"/>
+      <c r="BF8" s="0"/>
+      <c r="BG8" s="0"/>
+      <c r="BH8" s="0"/>
+      <c r="BI8" s="0"/>
+      <c r="BJ8" s="0"/>
+      <c r="BK8" s="0"/>
+      <c r="BL8" s="0"/>
+      <c r="BM8" s="0"/>
+      <c r="BN8" s="0"/>
+      <c r="BO8" s="0"/>
+      <c r="BP8" s="0"/>
+      <c r="BQ8" s="0"/>
+      <c r="BR8" s="0"/>
+      <c r="BS8" s="0"/>
+      <c r="BT8" s="0"/>
+      <c r="BU8" s="0"/>
+      <c r="BV8" s="0"/>
+      <c r="BW8" s="0"/>
+      <c r="BX8" s="0"/>
+      <c r="BY8" s="0"/>
+      <c r="BZ8" s="0"/>
+      <c r="CA8" s="0"/>
+      <c r="CB8" s="0"/>
+      <c r="CC8" s="0"/>
+      <c r="CD8" s="0"/>
+      <c r="CE8" s="0"/>
+      <c r="CF8" s="0"/>
+      <c r="CG8" s="0"/>
+      <c r="CH8" s="0"/>
+      <c r="CI8" s="0"/>
+      <c r="CJ8" s="0"/>
+      <c r="CK8" s="0"/>
+      <c r="CL8" s="0"/>
+      <c r="CM8" s="0"/>
+      <c r="CN8" s="0"/>
+      <c r="CO8" s="0"/>
+      <c r="CP8" s="0"/>
+      <c r="CQ8" s="0"/>
+      <c r="CR8" s="0"/>
+      <c r="CS8" s="0"/>
+      <c r="CT8" s="0"/>
+      <c r="CU8" s="0"/>
+      <c r="CV8" s="0"/>
+      <c r="CW8" s="0"/>
+      <c r="CX8" s="0"/>
+      <c r="CY8" s="0"/>
+      <c r="CZ8" s="0"/>
+      <c r="DA8" s="0"/>
+      <c r="DB8" s="0"/>
+      <c r="DC8" s="0"/>
+      <c r="DD8" s="0"/>
+      <c r="DE8" s="0"/>
+      <c r="DF8" s="0"/>
+      <c r="DG8" s="0"/>
+      <c r="DH8" s="0"/>
+      <c r="DI8" s="0"/>
+      <c r="DJ8" s="0"/>
+      <c r="DK8" s="0"/>
+      <c r="DL8" s="0"/>
+      <c r="DM8" s="0"/>
+      <c r="DN8" s="0"/>
+      <c r="DO8" s="0"/>
+      <c r="DP8" s="0"/>
+      <c r="DQ8" s="0"/>
+      <c r="DR8" s="0"/>
+      <c r="DS8" s="0"/>
+      <c r="DT8" s="0"/>
+      <c r="DU8" s="0"/>
+      <c r="DV8" s="0"/>
+      <c r="DW8" s="0"/>
+      <c r="DX8" s="0"/>
+      <c r="DY8" s="0"/>
+      <c r="DZ8" s="0"/>
+      <c r="EA8" s="0"/>
+      <c r="EB8" s="0"/>
+      <c r="EC8" s="0"/>
+      <c r="ED8" s="0"/>
+      <c r="EE8" s="0"/>
+      <c r="EF8" s="0"/>
+      <c r="EG8" s="0"/>
+      <c r="EH8" s="0"/>
+      <c r="EI8" s="0"/>
+      <c r="EJ8" s="0"/>
+      <c r="EK8" s="0"/>
+      <c r="EL8" s="0"/>
+      <c r="EM8" s="0"/>
+      <c r="EN8" s="0"/>
+      <c r="EO8" s="0"/>
+      <c r="EP8" s="0"/>
+      <c r="EQ8" s="0"/>
+      <c r="ER8" s="0"/>
+      <c r="ES8" s="0"/>
+      <c r="ET8" s="0"/>
+      <c r="EU8" s="0"/>
+      <c r="EV8" s="0"/>
+      <c r="EW8" s="0"/>
+      <c r="EX8" s="0"/>
+      <c r="EY8" s="0"/>
+      <c r="EZ8" s="0"/>
+      <c r="FA8" s="0"/>
+      <c r="FB8" s="0"/>
+      <c r="FC8" s="0"/>
+      <c r="FD8" s="0"/>
+      <c r="FE8" s="0"/>
+      <c r="FF8" s="0"/>
+      <c r="FG8" s="0"/>
+      <c r="FH8" s="0"/>
+      <c r="FI8" s="0"/>
+      <c r="FJ8" s="0"/>
+      <c r="FK8" s="0"/>
+      <c r="FL8" s="0"/>
+      <c r="FM8" s="0"/>
+      <c r="FN8" s="0"/>
+      <c r="FO8" s="0"/>
+      <c r="FP8" s="0"/>
+      <c r="FQ8" s="0"/>
+      <c r="FR8" s="0"/>
+      <c r="FS8" s="0"/>
+      <c r="FT8" s="0"/>
+      <c r="FU8" s="0"/>
+      <c r="FV8" s="0"/>
+      <c r="FW8" s="0"/>
+      <c r="FX8" s="0"/>
+      <c r="FY8" s="0"/>
+      <c r="FZ8" s="0"/>
+      <c r="GA8" s="0"/>
+      <c r="GB8" s="0"/>
+      <c r="GC8" s="0"/>
+      <c r="GD8" s="0"/>
+      <c r="GE8" s="0"/>
+      <c r="GF8" s="0"/>
+      <c r="GG8" s="0"/>
+      <c r="GH8" s="0"/>
+      <c r="GI8" s="0"/>
+      <c r="GJ8" s="0"/>
+      <c r="GK8" s="0"/>
+      <c r="GL8" s="0"/>
+      <c r="GM8" s="0"/>
+      <c r="GN8" s="0"/>
+      <c r="GO8" s="0"/>
+      <c r="GP8" s="0"/>
+      <c r="GQ8" s="0"/>
+      <c r="GR8" s="0"/>
+      <c r="GS8" s="0"/>
+      <c r="GT8" s="0"/>
+      <c r="GU8" s="0"/>
+      <c r="GV8" s="0"/>
+      <c r="GW8" s="0"/>
+      <c r="GX8" s="0"/>
+      <c r="GY8" s="0"/>
+      <c r="GZ8" s="0"/>
+      <c r="HA8" s="0"/>
+      <c r="HB8" s="0"/>
+      <c r="HC8" s="0"/>
+      <c r="HD8" s="0"/>
+      <c r="HE8" s="0"/>
+      <c r="HF8" s="0"/>
+      <c r="HG8" s="0"/>
+      <c r="HH8" s="0"/>
+      <c r="HI8" s="0"/>
+      <c r="HJ8" s="0"/>
+      <c r="HK8" s="0"/>
+      <c r="HL8" s="0"/>
+      <c r="HM8" s="0"/>
+      <c r="HN8" s="0"/>
+      <c r="HO8" s="0"/>
+      <c r="HP8" s="0"/>
+      <c r="HQ8" s="0"/>
+      <c r="HR8" s="0"/>
+      <c r="HS8" s="0"/>
+      <c r="HT8" s="0"/>
+      <c r="HU8" s="0"/>
+      <c r="HV8" s="0"/>
+      <c r="HW8" s="0"/>
+      <c r="HX8" s="0"/>
+      <c r="HY8" s="0"/>
+      <c r="HZ8" s="0"/>
+      <c r="IA8" s="0"/>
+      <c r="IB8" s="0"/>
+      <c r="IC8" s="0"/>
+      <c r="ID8" s="0"/>
+      <c r="IE8" s="0"/>
+      <c r="IF8" s="0"/>
+      <c r="IG8" s="0"/>
+      <c r="IH8" s="0"/>
+      <c r="II8" s="0"/>
+      <c r="IJ8" s="0"/>
+      <c r="IK8" s="0"/>
+      <c r="IL8" s="0"/>
+      <c r="IM8" s="0"/>
+      <c r="IN8" s="0"/>
+      <c r="IO8" s="0"/>
+      <c r="IP8" s="0"/>
+      <c r="IQ8" s="0"/>
+      <c r="IR8" s="0"/>
+      <c r="IS8" s="0"/>
+      <c r="IT8" s="0"/>
+      <c r="IU8" s="0"/>
+      <c r="IV8" s="0"/>
+      <c r="IW8" s="0"/>
+      <c r="IX8" s="0"/>
+      <c r="IY8" s="0"/>
+      <c r="IZ8" s="0"/>
+      <c r="JA8" s="0"/>
+      <c r="JB8" s="0"/>
+      <c r="JC8" s="0"/>
+      <c r="JD8" s="0"/>
+      <c r="JE8" s="0"/>
+      <c r="JF8" s="0"/>
+      <c r="JG8" s="0"/>
+      <c r="JH8" s="0"/>
+      <c r="JI8" s="0"/>
+      <c r="JJ8" s="0"/>
+      <c r="JK8" s="0"/>
+      <c r="JL8" s="0"/>
+      <c r="JM8" s="0"/>
+      <c r="JN8" s="0"/>
+      <c r="JO8" s="0"/>
+      <c r="JP8" s="0"/>
+      <c r="JQ8" s="0"/>
+      <c r="JR8" s="0"/>
+      <c r="JS8" s="0"/>
+      <c r="JT8" s="0"/>
+      <c r="JU8" s="0"/>
+      <c r="JV8" s="0"/>
+      <c r="JW8" s="0"/>
+      <c r="JX8" s="0"/>
+      <c r="JY8" s="0"/>
+      <c r="JZ8" s="0"/>
+      <c r="KA8" s="0"/>
+      <c r="KB8" s="0"/>
+      <c r="KC8" s="0"/>
+      <c r="KD8" s="0"/>
+      <c r="KE8" s="0"/>
+      <c r="KF8" s="0"/>
+      <c r="KG8" s="0"/>
+      <c r="KH8" s="0"/>
+      <c r="KI8" s="0"/>
+      <c r="KJ8" s="0"/>
+      <c r="KK8" s="0"/>
+      <c r="KL8" s="0"/>
+      <c r="KM8" s="0"/>
+      <c r="KN8" s="0"/>
+      <c r="KO8" s="0"/>
+      <c r="KP8" s="0"/>
+      <c r="KQ8" s="0"/>
+      <c r="KR8" s="0"/>
+      <c r="KS8" s="0"/>
+      <c r="KT8" s="0"/>
+      <c r="KU8" s="0"/>
+      <c r="KV8" s="0"/>
+      <c r="KW8" s="0"/>
+      <c r="KX8" s="0"/>
+      <c r="KY8" s="0"/>
+      <c r="KZ8" s="0"/>
+      <c r="LA8" s="0"/>
+      <c r="LB8" s="0"/>
+      <c r="LC8" s="0"/>
+      <c r="LD8" s="0"/>
+      <c r="LE8" s="0"/>
+      <c r="LF8" s="0"/>
+      <c r="LG8" s="0"/>
+      <c r="LH8" s="0"/>
+      <c r="LI8" s="0"/>
+      <c r="LJ8" s="0"/>
+      <c r="LK8" s="0"/>
+      <c r="LL8" s="0"/>
+      <c r="LM8" s="0"/>
+      <c r="LN8" s="0"/>
+      <c r="LO8" s="0"/>
+      <c r="LP8" s="0"/>
+      <c r="LQ8" s="0"/>
+      <c r="LR8" s="0"/>
+      <c r="LS8" s="0"/>
+      <c r="LT8" s="0"/>
+      <c r="LU8" s="0"/>
+      <c r="LV8" s="0"/>
+      <c r="LW8" s="0"/>
+      <c r="LX8" s="0"/>
+      <c r="LY8" s="0"/>
+      <c r="LZ8" s="0"/>
+      <c r="MA8" s="0"/>
+      <c r="MB8" s="0"/>
+      <c r="MC8" s="0"/>
+      <c r="MD8" s="0"/>
+      <c r="ME8" s="0"/>
+      <c r="MF8" s="0"/>
+      <c r="MG8" s="0"/>
+      <c r="MH8" s="0"/>
+      <c r="MI8" s="0"/>
+      <c r="MJ8" s="0"/>
+      <c r="MK8" s="0"/>
+      <c r="ML8" s="0"/>
+      <c r="MM8" s="0"/>
+      <c r="MN8" s="0"/>
+      <c r="MO8" s="0"/>
+      <c r="MP8" s="0"/>
+      <c r="MQ8" s="0"/>
+      <c r="MR8" s="0"/>
+      <c r="MS8" s="0"/>
+      <c r="MT8" s="0"/>
+      <c r="MU8" s="0"/>
+      <c r="MV8" s="0"/>
+      <c r="MW8" s="0"/>
+      <c r="MX8" s="0"/>
+      <c r="MY8" s="0"/>
+      <c r="MZ8" s="0"/>
+      <c r="NA8" s="0"/>
+      <c r="NB8" s="0"/>
+      <c r="NC8" s="0"/>
+      <c r="ND8" s="0"/>
+      <c r="NE8" s="0"/>
+      <c r="NF8" s="0"/>
+      <c r="NG8" s="0"/>
+      <c r="NH8" s="0"/>
+      <c r="NI8" s="0"/>
+      <c r="NJ8" s="0"/>
+      <c r="NK8" s="0"/>
+      <c r="NL8" s="0"/>
+      <c r="NM8" s="0"/>
+      <c r="NN8" s="0"/>
+      <c r="NO8" s="0"/>
+      <c r="NP8" s="0"/>
+      <c r="NQ8" s="0"/>
+      <c r="NR8" s="0"/>
+      <c r="NS8" s="0"/>
+      <c r="NT8" s="0"/>
+      <c r="NU8" s="0"/>
+      <c r="NV8" s="0"/>
+      <c r="NW8" s="0"/>
+      <c r="NX8" s="0"/>
+      <c r="NY8" s="0"/>
+      <c r="NZ8" s="0"/>
+      <c r="OA8" s="0"/>
+      <c r="OB8" s="0"/>
+      <c r="OC8" s="0"/>
+      <c r="OD8" s="0"/>
+      <c r="OE8" s="0"/>
+      <c r="OF8" s="0"/>
+      <c r="OG8" s="0"/>
+      <c r="OH8" s="0"/>
+      <c r="OI8" s="0"/>
+      <c r="OJ8" s="0"/>
+      <c r="OK8" s="0"/>
+      <c r="OL8" s="0"/>
+      <c r="OM8" s="0"/>
+      <c r="ON8" s="0"/>
+      <c r="OO8" s="0"/>
+      <c r="OP8" s="0"/>
+      <c r="OQ8" s="0"/>
+      <c r="OR8" s="0"/>
+      <c r="OS8" s="0"/>
+      <c r="OT8" s="0"/>
+      <c r="OU8" s="0"/>
+      <c r="OV8" s="0"/>
+      <c r="OW8" s="0"/>
+      <c r="OX8" s="0"/>
+      <c r="OY8" s="0"/>
+      <c r="OZ8" s="0"/>
+      <c r="PA8" s="0"/>
+      <c r="PB8" s="0"/>
+      <c r="PC8" s="0"/>
+      <c r="PD8" s="0"/>
+      <c r="PE8" s="0"/>
+      <c r="PF8" s="0"/>
+      <c r="PG8" s="0"/>
+      <c r="PH8" s="0"/>
+      <c r="PI8" s="0"/>
+      <c r="PJ8" s="0"/>
+      <c r="PK8" s="0"/>
+      <c r="PL8" s="0"/>
+      <c r="PM8" s="0"/>
+      <c r="PN8" s="0"/>
+      <c r="PO8" s="0"/>
+      <c r="PP8" s="0"/>
+      <c r="PQ8" s="0"/>
+      <c r="PR8" s="0"/>
+      <c r="PS8" s="0"/>
+      <c r="PT8" s="0"/>
+      <c r="PU8" s="0"/>
+      <c r="PV8" s="0"/>
+      <c r="PW8" s="0"/>
+      <c r="PX8" s="0"/>
+      <c r="PY8" s="0"/>
+      <c r="PZ8" s="0"/>
+      <c r="QA8" s="0"/>
+      <c r="QB8" s="0"/>
+      <c r="QC8" s="0"/>
+      <c r="QD8" s="0"/>
+      <c r="QE8" s="0"/>
+      <c r="QF8" s="0"/>
+      <c r="QG8" s="0"/>
+      <c r="QH8" s="0"/>
+      <c r="QI8" s="0"/>
+      <c r="QJ8" s="0"/>
+      <c r="QK8" s="0"/>
+      <c r="QL8" s="0"/>
+      <c r="QM8" s="0"/>
+      <c r="QN8" s="0"/>
+      <c r="QO8" s="0"/>
+      <c r="QP8" s="0"/>
+      <c r="QQ8" s="0"/>
+      <c r="QR8" s="0"/>
+      <c r="QS8" s="0"/>
+      <c r="QT8" s="0"/>
+      <c r="QU8" s="0"/>
+      <c r="QV8" s="0"/>
+      <c r="QW8" s="0"/>
+      <c r="QX8" s="0"/>
+      <c r="QY8" s="0"/>
+      <c r="QZ8" s="0"/>
+      <c r="RA8" s="0"/>
+      <c r="RB8" s="0"/>
+      <c r="RC8" s="0"/>
+      <c r="RD8" s="0"/>
+      <c r="RE8" s="0"/>
+      <c r="RF8" s="0"/>
+      <c r="RG8" s="0"/>
+      <c r="RH8" s="0"/>
+      <c r="RI8" s="0"/>
+      <c r="RJ8" s="0"/>
+      <c r="RK8" s="0"/>
+      <c r="RL8" s="0"/>
+      <c r="RM8" s="0"/>
+      <c r="RN8" s="0"/>
+      <c r="RO8" s="0"/>
+      <c r="RP8" s="0"/>
+      <c r="RQ8" s="0"/>
+      <c r="RR8" s="0"/>
+      <c r="RS8" s="0"/>
+      <c r="RT8" s="0"/>
+      <c r="RU8" s="0"/>
+      <c r="RV8" s="0"/>
+      <c r="RW8" s="0"/>
+      <c r="RX8" s="0"/>
+      <c r="RY8" s="0"/>
+      <c r="RZ8" s="0"/>
+      <c r="SA8" s="0"/>
+      <c r="SB8" s="0"/>
+      <c r="SC8" s="0"/>
+      <c r="SD8" s="0"/>
+      <c r="SE8" s="0"/>
+      <c r="SF8" s="0"/>
+      <c r="SG8" s="0"/>
+      <c r="SH8" s="0"/>
+      <c r="SI8" s="0"/>
+      <c r="SJ8" s="0"/>
+      <c r="SK8" s="0"/>
+      <c r="SL8" s="0"/>
+      <c r="SM8" s="0"/>
+      <c r="SN8" s="0"/>
+      <c r="SO8" s="0"/>
+      <c r="SP8" s="0"/>
+      <c r="SQ8" s="0"/>
+      <c r="SR8" s="0"/>
+      <c r="SS8" s="0"/>
+      <c r="ST8" s="0"/>
+      <c r="SU8" s="0"/>
+      <c r="SV8" s="0"/>
+      <c r="SW8" s="0"/>
+      <c r="SX8" s="0"/>
+      <c r="SY8" s="0"/>
+      <c r="SZ8" s="0"/>
+      <c r="TA8" s="0"/>
+      <c r="TB8" s="0"/>
+      <c r="TC8" s="0"/>
+      <c r="TD8" s="0"/>
+      <c r="TE8" s="0"/>
+      <c r="TF8" s="0"/>
+      <c r="TG8" s="0"/>
+      <c r="TH8" s="0"/>
+      <c r="TI8" s="0"/>
+      <c r="TJ8" s="0"/>
+      <c r="TK8" s="0"/>
+      <c r="TL8" s="0"/>
+      <c r="TM8" s="0"/>
+      <c r="TN8" s="0"/>
+      <c r="TO8" s="0"/>
+      <c r="TP8" s="0"/>
+      <c r="TQ8" s="0"/>
+      <c r="TR8" s="0"/>
+      <c r="TS8" s="0"/>
+      <c r="TT8" s="0"/>
+      <c r="TU8" s="0"/>
+      <c r="TV8" s="0"/>
+      <c r="TW8" s="0"/>
+      <c r="TX8" s="0"/>
+      <c r="TY8" s="0"/>
+      <c r="TZ8" s="0"/>
+      <c r="UA8" s="0"/>
+      <c r="UB8" s="0"/>
+      <c r="UC8" s="0"/>
+      <c r="UD8" s="0"/>
+      <c r="UE8" s="0"/>
+      <c r="UF8" s="0"/>
+      <c r="UG8" s="0"/>
+      <c r="UH8" s="0"/>
+      <c r="UI8" s="0"/>
+      <c r="UJ8" s="0"/>
+      <c r="UK8" s="0"/>
+      <c r="UL8" s="0"/>
+      <c r="UM8" s="0"/>
+      <c r="UN8" s="0"/>
+      <c r="UO8" s="0"/>
+      <c r="UP8" s="0"/>
+      <c r="UQ8" s="0"/>
+      <c r="UR8" s="0"/>
+      <c r="US8" s="0"/>
+      <c r="UT8" s="0"/>
+      <c r="UU8" s="0"/>
+      <c r="UV8" s="0"/>
+      <c r="UW8" s="0"/>
+      <c r="UX8" s="0"/>
+      <c r="UY8" s="0"/>
+      <c r="UZ8" s="0"/>
+      <c r="VA8" s="0"/>
+      <c r="VB8" s="0"/>
+      <c r="VC8" s="0"/>
+      <c r="VD8" s="0"/>
+      <c r="VE8" s="0"/>
+      <c r="VF8" s="0"/>
+      <c r="VG8" s="0"/>
+      <c r="VH8" s="0"/>
+      <c r="VI8" s="0"/>
+      <c r="VJ8" s="0"/>
+      <c r="VK8" s="0"/>
+      <c r="VL8" s="0"/>
+      <c r="VM8" s="0"/>
+      <c r="VN8" s="0"/>
+      <c r="VO8" s="0"/>
+      <c r="VP8" s="0"/>
+      <c r="VQ8" s="0"/>
+      <c r="VR8" s="0"/>
+      <c r="VS8" s="0"/>
+      <c r="VT8" s="0"/>
+      <c r="VU8" s="0"/>
+      <c r="VV8" s="0"/>
+      <c r="VW8" s="0"/>
+      <c r="VX8" s="0"/>
+      <c r="VY8" s="0"/>
+      <c r="VZ8" s="0"/>
+      <c r="WA8" s="0"/>
+      <c r="WB8" s="0"/>
+      <c r="WC8" s="0"/>
+      <c r="WD8" s="0"/>
+      <c r="WE8" s="0"/>
+      <c r="WF8" s="0"/>
+      <c r="WG8" s="0"/>
+      <c r="WH8" s="0"/>
+      <c r="WI8" s="0"/>
+      <c r="WJ8" s="0"/>
+      <c r="WK8" s="0"/>
+      <c r="WL8" s="0"/>
+      <c r="WM8" s="0"/>
+      <c r="WN8" s="0"/>
+      <c r="WO8" s="0"/>
+      <c r="WP8" s="0"/>
+      <c r="WQ8" s="0"/>
+      <c r="WR8" s="0"/>
+      <c r="WS8" s="0"/>
+      <c r="WT8" s="0"/>
+      <c r="WU8" s="0"/>
+      <c r="WV8" s="0"/>
+      <c r="WW8" s="0"/>
+      <c r="WX8" s="0"/>
+      <c r="WY8" s="0"/>
+      <c r="WZ8" s="0"/>
+      <c r="XA8" s="0"/>
+      <c r="XB8" s="0"/>
+      <c r="XC8" s="0"/>
+      <c r="XD8" s="0"/>
+      <c r="XE8" s="0"/>
+      <c r="XF8" s="0"/>
+      <c r="XG8" s="0"/>
+      <c r="XH8" s="0"/>
+      <c r="XI8" s="0"/>
+      <c r="XJ8" s="0"/>
+      <c r="XK8" s="0"/>
+      <c r="XL8" s="0"/>
+      <c r="XM8" s="0"/>
+      <c r="XN8" s="0"/>
+      <c r="XO8" s="0"/>
+      <c r="XP8" s="0"/>
+      <c r="XQ8" s="0"/>
+      <c r="XR8" s="0"/>
+      <c r="XS8" s="0"/>
+      <c r="XT8" s="0"/>
+      <c r="XU8" s="0"/>
+      <c r="XV8" s="0"/>
+      <c r="XW8" s="0"/>
+      <c r="XX8" s="0"/>
+      <c r="XY8" s="0"/>
+      <c r="XZ8" s="0"/>
+      <c r="YA8" s="0"/>
+      <c r="YB8" s="0"/>
+      <c r="YC8" s="0"/>
+      <c r="YD8" s="0"/>
+      <c r="YE8" s="0"/>
+      <c r="YF8" s="0"/>
+      <c r="YG8" s="0"/>
+      <c r="YH8" s="0"/>
+      <c r="YI8" s="0"/>
+      <c r="YJ8" s="0"/>
+      <c r="YK8" s="0"/>
+      <c r="YL8" s="0"/>
+      <c r="YM8" s="0"/>
+      <c r="YN8" s="0"/>
+      <c r="YO8" s="0"/>
+      <c r="YP8" s="0"/>
+      <c r="YQ8" s="0"/>
+      <c r="YR8" s="0"/>
+      <c r="YS8" s="0"/>
+      <c r="YT8" s="0"/>
+      <c r="YU8" s="0"/>
+      <c r="YV8" s="0"/>
+      <c r="YW8" s="0"/>
+      <c r="YX8" s="0"/>
+      <c r="YY8" s="0"/>
+      <c r="YZ8" s="0"/>
+      <c r="ZA8" s="0"/>
+      <c r="ZB8" s="0"/>
+      <c r="ZC8" s="0"/>
+      <c r="ZD8" s="0"/>
+      <c r="ZE8" s="0"/>
+      <c r="ZF8" s="0"/>
+      <c r="ZG8" s="0"/>
+      <c r="ZH8" s="0"/>
+      <c r="ZI8" s="0"/>
+      <c r="ZJ8" s="0"/>
+      <c r="ZK8" s="0"/>
+      <c r="ZL8" s="0"/>
+      <c r="ZM8" s="0"/>
+      <c r="ZN8" s="0"/>
+      <c r="ZO8" s="0"/>
+      <c r="ZP8" s="0"/>
+      <c r="ZQ8" s="0"/>
+      <c r="ZR8" s="0"/>
+      <c r="ZS8" s="0"/>
+      <c r="ZT8" s="0"/>
+      <c r="ZU8" s="0"/>
+      <c r="ZV8" s="0"/>
+      <c r="ZW8" s="0"/>
+      <c r="ZX8" s="0"/>
+      <c r="ZY8" s="0"/>
+      <c r="ZZ8" s="0"/>
+      <c r="AAA8" s="0"/>
+      <c r="AAB8" s="0"/>
+      <c r="AAC8" s="0"/>
+      <c r="AAD8" s="0"/>
+      <c r="AAE8" s="0"/>
+      <c r="AAF8" s="0"/>
+      <c r="AAG8" s="0"/>
+      <c r="AAH8" s="0"/>
+      <c r="AAI8" s="0"/>
+      <c r="AAJ8" s="0"/>
+      <c r="AAK8" s="0"/>
+      <c r="AAL8" s="0"/>
+      <c r="AAM8" s="0"/>
+      <c r="AAN8" s="0"/>
+      <c r="AAO8" s="0"/>
+      <c r="AAP8" s="0"/>
+      <c r="AAQ8" s="0"/>
+      <c r="AAR8" s="0"/>
+      <c r="AAS8" s="0"/>
+      <c r="AAT8" s="0"/>
+      <c r="AAU8" s="0"/>
+      <c r="AAV8" s="0"/>
+      <c r="AAW8" s="0"/>
+      <c r="AAX8" s="0"/>
+      <c r="AAY8" s="0"/>
+      <c r="AAZ8" s="0"/>
+      <c r="ABA8" s="0"/>
+      <c r="ABB8" s="0"/>
+      <c r="ABC8" s="0"/>
+      <c r="ABD8" s="0"/>
+      <c r="ABE8" s="0"/>
+      <c r="ABF8" s="0"/>
+      <c r="ABG8" s="0"/>
+      <c r="ABH8" s="0"/>
+      <c r="ABI8" s="0"/>
+      <c r="ABJ8" s="0"/>
+      <c r="ABK8" s="0"/>
+      <c r="ABL8" s="0"/>
+      <c r="ABM8" s="0"/>
+      <c r="ABN8" s="0"/>
+      <c r="ABO8" s="0"/>
+      <c r="ABP8" s="0"/>
+      <c r="ABQ8" s="0"/>
+      <c r="ABR8" s="0"/>
+      <c r="ABS8" s="0"/>
+      <c r="ABT8" s="0"/>
+      <c r="ABU8" s="0"/>
+      <c r="ABV8" s="0"/>
+      <c r="ABW8" s="0"/>
+      <c r="ABX8" s="0"/>
+      <c r="ABY8" s="0"/>
+      <c r="ABZ8" s="0"/>
+      <c r="ACA8" s="0"/>
+      <c r="ACB8" s="0"/>
+      <c r="ACC8" s="0"/>
+      <c r="ACD8" s="0"/>
+      <c r="ACE8" s="0"/>
+      <c r="ACF8" s="0"/>
+      <c r="ACG8" s="0"/>
+      <c r="ACH8" s="0"/>
+      <c r="ACI8" s="0"/>
+      <c r="ACJ8" s="0"/>
+      <c r="ACK8" s="0"/>
+      <c r="ACL8" s="0"/>
+      <c r="ACM8" s="0"/>
+      <c r="ACN8" s="0"/>
+      <c r="ACO8" s="0"/>
+      <c r="ACP8" s="0"/>
+      <c r="ACQ8" s="0"/>
+      <c r="ACR8" s="0"/>
+      <c r="ACS8" s="0"/>
+      <c r="ACT8" s="0"/>
+      <c r="ACU8" s="0"/>
+      <c r="ACV8" s="0"/>
+      <c r="ACW8" s="0"/>
+      <c r="ACX8" s="0"/>
+      <c r="ACY8" s="0"/>
+      <c r="ACZ8" s="0"/>
+      <c r="ADA8" s="0"/>
+      <c r="ADB8" s="0"/>
+      <c r="ADC8" s="0"/>
+      <c r="ADD8" s="0"/>
+      <c r="ADE8" s="0"/>
+      <c r="ADF8" s="0"/>
+      <c r="ADG8" s="0"/>
+      <c r="ADH8" s="0"/>
+      <c r="ADI8" s="0"/>
+      <c r="ADJ8" s="0"/>
+      <c r="ADK8" s="0"/>
+      <c r="ADL8" s="0"/>
+      <c r="ADM8" s="0"/>
+      <c r="ADN8" s="0"/>
+      <c r="ADO8" s="0"/>
+      <c r="ADP8" s="0"/>
+      <c r="ADQ8" s="0"/>
+      <c r="ADR8" s="0"/>
+      <c r="ADS8" s="0"/>
+      <c r="ADT8" s="0"/>
+      <c r="ADU8" s="0"/>
+      <c r="ADV8" s="0"/>
+      <c r="ADW8" s="0"/>
+      <c r="ADX8" s="0"/>
+      <c r="ADY8" s="0"/>
+      <c r="ADZ8" s="0"/>
+      <c r="AEA8" s="0"/>
+      <c r="AEB8" s="0"/>
+      <c r="AEC8" s="0"/>
+      <c r="AED8" s="0"/>
+      <c r="AEE8" s="0"/>
+      <c r="AEF8" s="0"/>
+      <c r="AEG8" s="0"/>
+      <c r="AEH8" s="0"/>
+      <c r="AEI8" s="0"/>
+      <c r="AEJ8" s="0"/>
+      <c r="AEK8" s="0"/>
+      <c r="AEL8" s="0"/>
+      <c r="AEM8" s="0"/>
+      <c r="AEN8" s="0"/>
+      <c r="AEO8" s="0"/>
+      <c r="AEP8" s="0"/>
+      <c r="AEQ8" s="0"/>
+      <c r="AER8" s="0"/>
+      <c r="AES8" s="0"/>
+      <c r="AET8" s="0"/>
+      <c r="AEU8" s="0"/>
+      <c r="AEV8" s="0"/>
+      <c r="AEW8" s="0"/>
+      <c r="AEX8" s="0"/>
+      <c r="AEY8" s="0"/>
+      <c r="AEZ8" s="0"/>
+      <c r="AFA8" s="0"/>
+      <c r="AFB8" s="0"/>
+      <c r="AFC8" s="0"/>
+      <c r="AFD8" s="0"/>
+      <c r="AFE8" s="0"/>
+      <c r="AFF8" s="0"/>
+      <c r="AFG8" s="0"/>
+      <c r="AFH8" s="0"/>
+      <c r="AFI8" s="0"/>
+      <c r="AFJ8" s="0"/>
+      <c r="AFK8" s="0"/>
+      <c r="AFL8" s="0"/>
+      <c r="AFM8" s="0"/>
+      <c r="AFN8" s="0"/>
+      <c r="AFO8" s="0"/>
+      <c r="AFP8" s="0"/>
+      <c r="AFQ8" s="0"/>
+      <c r="AFR8" s="0"/>
+      <c r="AFS8" s="0"/>
+      <c r="AFT8" s="0"/>
+      <c r="AFU8" s="0"/>
+      <c r="AFV8" s="0"/>
+      <c r="AFW8" s="0"/>
+      <c r="AFX8" s="0"/>
+      <c r="AFY8" s="0"/>
+      <c r="AFZ8" s="0"/>
+      <c r="AGA8" s="0"/>
+      <c r="AGB8" s="0"/>
+      <c r="AGC8" s="0"/>
+      <c r="AGD8" s="0"/>
+      <c r="AGE8" s="0"/>
+      <c r="AGF8" s="0"/>
+      <c r="AGG8" s="0"/>
+      <c r="AGH8" s="0"/>
+      <c r="AGI8" s="0"/>
+      <c r="AGJ8" s="0"/>
+      <c r="AGK8" s="0"/>
+      <c r="AGL8" s="0"/>
+      <c r="AGM8" s="0"/>
+      <c r="AGN8" s="0"/>
+      <c r="AGO8" s="0"/>
+      <c r="AGP8" s="0"/>
+      <c r="AGQ8" s="0"/>
+      <c r="AGR8" s="0"/>
+      <c r="AGS8" s="0"/>
+      <c r="AGT8" s="0"/>
+      <c r="AGU8" s="0"/>
+      <c r="AGV8" s="0"/>
+      <c r="AGW8" s="0"/>
+      <c r="AGX8" s="0"/>
+      <c r="AGY8" s="0"/>
+      <c r="AGZ8" s="0"/>
+      <c r="AHA8" s="0"/>
+      <c r="AHB8" s="0"/>
+      <c r="AHC8" s="0"/>
+      <c r="AHD8" s="0"/>
+      <c r="AHE8" s="0"/>
+      <c r="AHF8" s="0"/>
+      <c r="AHG8" s="0"/>
+      <c r="AHH8" s="0"/>
+      <c r="AHI8" s="0"/>
+      <c r="AHJ8" s="0"/>
+      <c r="AHK8" s="0"/>
+      <c r="AHL8" s="0"/>
+      <c r="AHM8" s="0"/>
+      <c r="AHN8" s="0"/>
+      <c r="AHO8" s="0"/>
+      <c r="AHP8" s="0"/>
+      <c r="AHQ8" s="0"/>
+      <c r="AHR8" s="0"/>
+      <c r="AHS8" s="0"/>
+      <c r="AHT8" s="0"/>
+      <c r="AHU8" s="0"/>
+      <c r="AHV8" s="0"/>
+      <c r="AHW8" s="0"/>
+      <c r="AHX8" s="0"/>
+      <c r="AHY8" s="0"/>
+      <c r="AHZ8" s="0"/>
+      <c r="AIA8" s="0"/>
+      <c r="AIB8" s="0"/>
+      <c r="AIC8" s="0"/>
+      <c r="AID8" s="0"/>
+      <c r="AIE8" s="0"/>
+      <c r="AIF8" s="0"/>
+      <c r="AIG8" s="0"/>
+      <c r="AIH8" s="0"/>
+      <c r="AII8" s="0"/>
+      <c r="AIJ8" s="0"/>
+      <c r="AIK8" s="0"/>
+      <c r="AIL8" s="0"/>
+      <c r="AIM8" s="0"/>
+      <c r="AIN8" s="0"/>
+      <c r="AIO8" s="0"/>
+      <c r="AIP8" s="0"/>
+      <c r="AIQ8" s="0"/>
+      <c r="AIR8" s="0"/>
+      <c r="AIS8" s="0"/>
+      <c r="AIT8" s="0"/>
+      <c r="AIU8" s="0"/>
+      <c r="AIV8" s="0"/>
+      <c r="AIW8" s="0"/>
+      <c r="AIX8" s="0"/>
+      <c r="AIY8" s="0"/>
+      <c r="AIZ8" s="0"/>
+      <c r="AJA8" s="0"/>
+      <c r="AJB8" s="0"/>
+      <c r="AJC8" s="0"/>
+      <c r="AJD8" s="0"/>
+      <c r="AJE8" s="0"/>
+      <c r="AJF8" s="0"/>
+      <c r="AJG8" s="0"/>
+      <c r="AJH8" s="0"/>
+      <c r="AJI8" s="0"/>
+      <c r="AJJ8" s="0"/>
+      <c r="AJK8" s="0"/>
+      <c r="AJL8" s="0"/>
+      <c r="AJM8" s="0"/>
+      <c r="AJN8" s="0"/>
+      <c r="AJO8" s="0"/>
+      <c r="AJP8" s="0"/>
+      <c r="AJQ8" s="0"/>
+      <c r="AJR8" s="0"/>
+      <c r="AJS8" s="0"/>
+      <c r="AJT8" s="0"/>
+      <c r="AJU8" s="0"/>
+      <c r="AJV8" s="0"/>
+      <c r="AJW8" s="0"/>
+      <c r="AJX8" s="0"/>
+      <c r="AJY8" s="0"/>
+      <c r="AJZ8" s="0"/>
+      <c r="AKA8" s="0"/>
+      <c r="AKB8" s="0"/>
+      <c r="AKC8" s="0"/>
+      <c r="AKD8" s="0"/>
+      <c r="AKE8" s="0"/>
+      <c r="AKF8" s="0"/>
+      <c r="AKG8" s="0"/>
+      <c r="AKH8" s="0"/>
+      <c r="AKI8" s="0"/>
+      <c r="AKJ8" s="0"/>
+      <c r="AKK8" s="0"/>
+      <c r="AKL8" s="0"/>
+      <c r="AKM8" s="0"/>
+      <c r="AKN8" s="0"/>
+      <c r="AKO8" s="0"/>
+      <c r="AKP8" s="0"/>
+      <c r="AKQ8" s="0"/>
+      <c r="AKR8" s="0"/>
+      <c r="AKS8" s="0"/>
+      <c r="AKT8" s="0"/>
+      <c r="AKU8" s="0"/>
+      <c r="AKV8" s="0"/>
+      <c r="AKW8" s="0"/>
+      <c r="AKX8" s="0"/>
+      <c r="AKY8" s="0"/>
+      <c r="AKZ8" s="0"/>
+      <c r="ALA8" s="0"/>
+      <c r="ALB8" s="0"/>
+      <c r="ALC8" s="0"/>
+      <c r="ALD8" s="0"/>
+      <c r="ALE8" s="0"/>
+      <c r="ALF8" s="0"/>
+      <c r="ALG8" s="0"/>
+      <c r="ALH8" s="0"/>
+      <c r="ALI8" s="0"/>
+      <c r="ALJ8" s="0"/>
+      <c r="ALK8" s="0"/>
+      <c r="ALL8" s="0"/>
+      <c r="ALM8" s="0"/>
+      <c r="ALN8" s="0"/>
+      <c r="ALO8" s="0"/>
+      <c r="ALP8" s="0"/>
+      <c r="ALQ8" s="0"/>
+      <c r="ALR8" s="0"/>
+      <c r="ALS8" s="0"/>
+      <c r="ALT8" s="0"/>
+      <c r="ALU8" s="0"/>
+      <c r="ALV8" s="0"/>
+      <c r="ALW8" s="0"/>
+      <c r="ALX8" s="0"/>
+      <c r="ALY8" s="0"/>
+      <c r="ALZ8" s="0"/>
+      <c r="AMA8" s="0"/>
+      <c r="AMB8" s="0"/>
+      <c r="AMC8" s="0"/>
+      <c r="AMD8" s="0"/>
+      <c r="AME8" s="0"/>
+      <c r="AMF8" s="0"/>
+      <c r="AMG8" s="0"/>
+      <c r="AMH8" s="0"/>
+      <c r="AMI8" s="0"/>
+      <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" s="24" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="20"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -3266,11 +4279,1025 @@
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
-      <c r="H9" s="22"/>
+      <c r="H9" s="20"/>
       <c r="I9" s="22"/>
-      <c r="J9" s="23"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
+      <c r="N9" s="0"/>
+      <c r="O9" s="0"/>
+      <c r="P9" s="0"/>
+      <c r="Q9" s="0"/>
+      <c r="R9" s="0"/>
+      <c r="S9" s="0"/>
+      <c r="T9" s="0"/>
+      <c r="U9" s="0"/>
+      <c r="V9" s="0"/>
+      <c r="W9" s="0"/>
+      <c r="X9" s="0"/>
+      <c r="Y9" s="0"/>
+      <c r="Z9" s="0"/>
+      <c r="AA9" s="0"/>
+      <c r="AB9" s="0"/>
+      <c r="AC9" s="0"/>
+      <c r="AD9" s="0"/>
+      <c r="AE9" s="0"/>
+      <c r="AF9" s="0"/>
+      <c r="AG9" s="0"/>
+      <c r="AH9" s="0"/>
+      <c r="AI9" s="0"/>
+      <c r="AJ9" s="0"/>
+      <c r="AK9" s="0"/>
+      <c r="AL9" s="0"/>
+      <c r="AM9" s="0"/>
+      <c r="AN9" s="0"/>
+      <c r="AO9" s="0"/>
+      <c r="AP9" s="0"/>
+      <c r="AQ9" s="0"/>
+      <c r="AR9" s="0"/>
+      <c r="AS9" s="0"/>
+      <c r="AT9" s="0"/>
+      <c r="AU9" s="0"/>
+      <c r="AV9" s="0"/>
+      <c r="AW9" s="0"/>
+      <c r="AX9" s="0"/>
+      <c r="AY9" s="0"/>
+      <c r="AZ9" s="0"/>
+      <c r="BA9" s="0"/>
+      <c r="BB9" s="0"/>
+      <c r="BC9" s="0"/>
+      <c r="BD9" s="0"/>
+      <c r="BE9" s="0"/>
+      <c r="BF9" s="0"/>
+      <c r="BG9" s="0"/>
+      <c r="BH9" s="0"/>
+      <c r="BI9" s="0"/>
+      <c r="BJ9" s="0"/>
+      <c r="BK9" s="0"/>
+      <c r="BL9" s="0"/>
+      <c r="BM9" s="0"/>
+      <c r="BN9" s="0"/>
+      <c r="BO9" s="0"/>
+      <c r="BP9" s="0"/>
+      <c r="BQ9" s="0"/>
+      <c r="BR9" s="0"/>
+      <c r="BS9" s="0"/>
+      <c r="BT9" s="0"/>
+      <c r="BU9" s="0"/>
+      <c r="BV9" s="0"/>
+      <c r="BW9" s="0"/>
+      <c r="BX9" s="0"/>
+      <c r="BY9" s="0"/>
+      <c r="BZ9" s="0"/>
+      <c r="CA9" s="0"/>
+      <c r="CB9" s="0"/>
+      <c r="CC9" s="0"/>
+      <c r="CD9" s="0"/>
+      <c r="CE9" s="0"/>
+      <c r="CF9" s="0"/>
+      <c r="CG9" s="0"/>
+      <c r="CH9" s="0"/>
+      <c r="CI9" s="0"/>
+      <c r="CJ9" s="0"/>
+      <c r="CK9" s="0"/>
+      <c r="CL9" s="0"/>
+      <c r="CM9" s="0"/>
+      <c r="CN9" s="0"/>
+      <c r="CO9" s="0"/>
+      <c r="CP9" s="0"/>
+      <c r="CQ9" s="0"/>
+      <c r="CR9" s="0"/>
+      <c r="CS9" s="0"/>
+      <c r="CT9" s="0"/>
+      <c r="CU9" s="0"/>
+      <c r="CV9" s="0"/>
+      <c r="CW9" s="0"/>
+      <c r="CX9" s="0"/>
+      <c r="CY9" s="0"/>
+      <c r="CZ9" s="0"/>
+      <c r="DA9" s="0"/>
+      <c r="DB9" s="0"/>
+      <c r="DC9" s="0"/>
+      <c r="DD9" s="0"/>
+      <c r="DE9" s="0"/>
+      <c r="DF9" s="0"/>
+      <c r="DG9" s="0"/>
+      <c r="DH9" s="0"/>
+      <c r="DI9" s="0"/>
+      <c r="DJ9" s="0"/>
+      <c r="DK9" s="0"/>
+      <c r="DL9" s="0"/>
+      <c r="DM9" s="0"/>
+      <c r="DN9" s="0"/>
+      <c r="DO9" s="0"/>
+      <c r="DP9" s="0"/>
+      <c r="DQ9" s="0"/>
+      <c r="DR9" s="0"/>
+      <c r="DS9" s="0"/>
+      <c r="DT9" s="0"/>
+      <c r="DU9" s="0"/>
+      <c r="DV9" s="0"/>
+      <c r="DW9" s="0"/>
+      <c r="DX9" s="0"/>
+      <c r="DY9" s="0"/>
+      <c r="DZ9" s="0"/>
+      <c r="EA9" s="0"/>
+      <c r="EB9" s="0"/>
+      <c r="EC9" s="0"/>
+      <c r="ED9" s="0"/>
+      <c r="EE9" s="0"/>
+      <c r="EF9" s="0"/>
+      <c r="EG9" s="0"/>
+      <c r="EH9" s="0"/>
+      <c r="EI9" s="0"/>
+      <c r="EJ9" s="0"/>
+      <c r="EK9" s="0"/>
+      <c r="EL9" s="0"/>
+      <c r="EM9" s="0"/>
+      <c r="EN9" s="0"/>
+      <c r="EO9" s="0"/>
+      <c r="EP9" s="0"/>
+      <c r="EQ9" s="0"/>
+      <c r="ER9" s="0"/>
+      <c r="ES9" s="0"/>
+      <c r="ET9" s="0"/>
+      <c r="EU9" s="0"/>
+      <c r="EV9" s="0"/>
+      <c r="EW9" s="0"/>
+      <c r="EX9" s="0"/>
+      <c r="EY9" s="0"/>
+      <c r="EZ9" s="0"/>
+      <c r="FA9" s="0"/>
+      <c r="FB9" s="0"/>
+      <c r="FC9" s="0"/>
+      <c r="FD9" s="0"/>
+      <c r="FE9" s="0"/>
+      <c r="FF9" s="0"/>
+      <c r="FG9" s="0"/>
+      <c r="FH9" s="0"/>
+      <c r="FI9" s="0"/>
+      <c r="FJ9" s="0"/>
+      <c r="FK9" s="0"/>
+      <c r="FL9" s="0"/>
+      <c r="FM9" s="0"/>
+      <c r="FN9" s="0"/>
+      <c r="FO9" s="0"/>
+      <c r="FP9" s="0"/>
+      <c r="FQ9" s="0"/>
+      <c r="FR9" s="0"/>
+      <c r="FS9" s="0"/>
+      <c r="FT9" s="0"/>
+      <c r="FU9" s="0"/>
+      <c r="FV9" s="0"/>
+      <c r="FW9" s="0"/>
+      <c r="FX9" s="0"/>
+      <c r="FY9" s="0"/>
+      <c r="FZ9" s="0"/>
+      <c r="GA9" s="0"/>
+      <c r="GB9" s="0"/>
+      <c r="GC9" s="0"/>
+      <c r="GD9" s="0"/>
+      <c r="GE9" s="0"/>
+      <c r="GF9" s="0"/>
+      <c r="GG9" s="0"/>
+      <c r="GH9" s="0"/>
+      <c r="GI9" s="0"/>
+      <c r="GJ9" s="0"/>
+      <c r="GK9" s="0"/>
+      <c r="GL9" s="0"/>
+      <c r="GM9" s="0"/>
+      <c r="GN9" s="0"/>
+      <c r="GO9" s="0"/>
+      <c r="GP9" s="0"/>
+      <c r="GQ9" s="0"/>
+      <c r="GR9" s="0"/>
+      <c r="GS9" s="0"/>
+      <c r="GT9" s="0"/>
+      <c r="GU9" s="0"/>
+      <c r="GV9" s="0"/>
+      <c r="GW9" s="0"/>
+      <c r="GX9" s="0"/>
+      <c r="GY9" s="0"/>
+      <c r="GZ9" s="0"/>
+      <c r="HA9" s="0"/>
+      <c r="HB9" s="0"/>
+      <c r="HC9" s="0"/>
+      <c r="HD9" s="0"/>
+      <c r="HE9" s="0"/>
+      <c r="HF9" s="0"/>
+      <c r="HG9" s="0"/>
+      <c r="HH9" s="0"/>
+      <c r="HI9" s="0"/>
+      <c r="HJ9" s="0"/>
+      <c r="HK9" s="0"/>
+      <c r="HL9" s="0"/>
+      <c r="HM9" s="0"/>
+      <c r="HN9" s="0"/>
+      <c r="HO9" s="0"/>
+      <c r="HP9" s="0"/>
+      <c r="HQ9" s="0"/>
+      <c r="HR9" s="0"/>
+      <c r="HS9" s="0"/>
+      <c r="HT9" s="0"/>
+      <c r="HU9" s="0"/>
+      <c r="HV9" s="0"/>
+      <c r="HW9" s="0"/>
+      <c r="HX9" s="0"/>
+      <c r="HY9" s="0"/>
+      <c r="HZ9" s="0"/>
+      <c r="IA9" s="0"/>
+      <c r="IB9" s="0"/>
+      <c r="IC9" s="0"/>
+      <c r="ID9" s="0"/>
+      <c r="IE9" s="0"/>
+      <c r="IF9" s="0"/>
+      <c r="IG9" s="0"/>
+      <c r="IH9" s="0"/>
+      <c r="II9" s="0"/>
+      <c r="IJ9" s="0"/>
+      <c r="IK9" s="0"/>
+      <c r="IL9" s="0"/>
+      <c r="IM9" s="0"/>
+      <c r="IN9" s="0"/>
+      <c r="IO9" s="0"/>
+      <c r="IP9" s="0"/>
+      <c r="IQ9" s="0"/>
+      <c r="IR9" s="0"/>
+      <c r="IS9" s="0"/>
+      <c r="IT9" s="0"/>
+      <c r="IU9" s="0"/>
+      <c r="IV9" s="0"/>
+      <c r="IW9" s="0"/>
+      <c r="IX9" s="0"/>
+      <c r="IY9" s="0"/>
+      <c r="IZ9" s="0"/>
+      <c r="JA9" s="0"/>
+      <c r="JB9" s="0"/>
+      <c r="JC9" s="0"/>
+      <c r="JD9" s="0"/>
+      <c r="JE9" s="0"/>
+      <c r="JF9" s="0"/>
+      <c r="JG9" s="0"/>
+      <c r="JH9" s="0"/>
+      <c r="JI9" s="0"/>
+      <c r="JJ9" s="0"/>
+      <c r="JK9" s="0"/>
+      <c r="JL9" s="0"/>
+      <c r="JM9" s="0"/>
+      <c r="JN9" s="0"/>
+      <c r="JO9" s="0"/>
+      <c r="JP9" s="0"/>
+      <c r="JQ9" s="0"/>
+      <c r="JR9" s="0"/>
+      <c r="JS9" s="0"/>
+      <c r="JT9" s="0"/>
+      <c r="JU9" s="0"/>
+      <c r="JV9" s="0"/>
+      <c r="JW9" s="0"/>
+      <c r="JX9" s="0"/>
+      <c r="JY9" s="0"/>
+      <c r="JZ9" s="0"/>
+      <c r="KA9" s="0"/>
+      <c r="KB9" s="0"/>
+      <c r="KC9" s="0"/>
+      <c r="KD9" s="0"/>
+      <c r="KE9" s="0"/>
+      <c r="KF9" s="0"/>
+      <c r="KG9" s="0"/>
+      <c r="KH9" s="0"/>
+      <c r="KI9" s="0"/>
+      <c r="KJ9" s="0"/>
+      <c r="KK9" s="0"/>
+      <c r="KL9" s="0"/>
+      <c r="KM9" s="0"/>
+      <c r="KN9" s="0"/>
+      <c r="KO9" s="0"/>
+      <c r="KP9" s="0"/>
+      <c r="KQ9" s="0"/>
+      <c r="KR9" s="0"/>
+      <c r="KS9" s="0"/>
+      <c r="KT9" s="0"/>
+      <c r="KU9" s="0"/>
+      <c r="KV9" s="0"/>
+      <c r="KW9" s="0"/>
+      <c r="KX9" s="0"/>
+      <c r="KY9" s="0"/>
+      <c r="KZ9" s="0"/>
+      <c r="LA9" s="0"/>
+      <c r="LB9" s="0"/>
+      <c r="LC9" s="0"/>
+      <c r="LD9" s="0"/>
+      <c r="LE9" s="0"/>
+      <c r="LF9" s="0"/>
+      <c r="LG9" s="0"/>
+      <c r="LH9" s="0"/>
+      <c r="LI9" s="0"/>
+      <c r="LJ9" s="0"/>
+      <c r="LK9" s="0"/>
+      <c r="LL9" s="0"/>
+      <c r="LM9" s="0"/>
+      <c r="LN9" s="0"/>
+      <c r="LO9" s="0"/>
+      <c r="LP9" s="0"/>
+      <c r="LQ9" s="0"/>
+      <c r="LR9" s="0"/>
+      <c r="LS9" s="0"/>
+      <c r="LT9" s="0"/>
+      <c r="LU9" s="0"/>
+      <c r="LV9" s="0"/>
+      <c r="LW9" s="0"/>
+      <c r="LX9" s="0"/>
+      <c r="LY9" s="0"/>
+      <c r="LZ9" s="0"/>
+      <c r="MA9" s="0"/>
+      <c r="MB9" s="0"/>
+      <c r="MC9" s="0"/>
+      <c r="MD9" s="0"/>
+      <c r="ME9" s="0"/>
+      <c r="MF9" s="0"/>
+      <c r="MG9" s="0"/>
+      <c r="MH9" s="0"/>
+      <c r="MI9" s="0"/>
+      <c r="MJ9" s="0"/>
+      <c r="MK9" s="0"/>
+      <c r="ML9" s="0"/>
+      <c r="MM9" s="0"/>
+      <c r="MN9" s="0"/>
+      <c r="MO9" s="0"/>
+      <c r="MP9" s="0"/>
+      <c r="MQ9" s="0"/>
+      <c r="MR9" s="0"/>
+      <c r="MS9" s="0"/>
+      <c r="MT9" s="0"/>
+      <c r="MU9" s="0"/>
+      <c r="MV9" s="0"/>
+      <c r="MW9" s="0"/>
+      <c r="MX9" s="0"/>
+      <c r="MY9" s="0"/>
+      <c r="MZ9" s="0"/>
+      <c r="NA9" s="0"/>
+      <c r="NB9" s="0"/>
+      <c r="NC9" s="0"/>
+      <c r="ND9" s="0"/>
+      <c r="NE9" s="0"/>
+      <c r="NF9" s="0"/>
+      <c r="NG9" s="0"/>
+      <c r="NH9" s="0"/>
+      <c r="NI9" s="0"/>
+      <c r="NJ9" s="0"/>
+      <c r="NK9" s="0"/>
+      <c r="NL9" s="0"/>
+      <c r="NM9" s="0"/>
+      <c r="NN9" s="0"/>
+      <c r="NO9" s="0"/>
+      <c r="NP9" s="0"/>
+      <c r="NQ9" s="0"/>
+      <c r="NR9" s="0"/>
+      <c r="NS9" s="0"/>
+      <c r="NT9" s="0"/>
+      <c r="NU9" s="0"/>
+      <c r="NV9" s="0"/>
+      <c r="NW9" s="0"/>
+      <c r="NX9" s="0"/>
+      <c r="NY9" s="0"/>
+      <c r="NZ9" s="0"/>
+      <c r="OA9" s="0"/>
+      <c r="OB9" s="0"/>
+      <c r="OC9" s="0"/>
+      <c r="OD9" s="0"/>
+      <c r="OE9" s="0"/>
+      <c r="OF9" s="0"/>
+      <c r="OG9" s="0"/>
+      <c r="OH9" s="0"/>
+      <c r="OI9" s="0"/>
+      <c r="OJ9" s="0"/>
+      <c r="OK9" s="0"/>
+      <c r="OL9" s="0"/>
+      <c r="OM9" s="0"/>
+      <c r="ON9" s="0"/>
+      <c r="OO9" s="0"/>
+      <c r="OP9" s="0"/>
+      <c r="OQ9" s="0"/>
+      <c r="OR9" s="0"/>
+      <c r="OS9" s="0"/>
+      <c r="OT9" s="0"/>
+      <c r="OU9" s="0"/>
+      <c r="OV9" s="0"/>
+      <c r="OW9" s="0"/>
+      <c r="OX9" s="0"/>
+      <c r="OY9" s="0"/>
+      <c r="OZ9" s="0"/>
+      <c r="PA9" s="0"/>
+      <c r="PB9" s="0"/>
+      <c r="PC9" s="0"/>
+      <c r="PD9" s="0"/>
+      <c r="PE9" s="0"/>
+      <c r="PF9" s="0"/>
+      <c r="PG9" s="0"/>
+      <c r="PH9" s="0"/>
+      <c r="PI9" s="0"/>
+      <c r="PJ9" s="0"/>
+      <c r="PK9" s="0"/>
+      <c r="PL9" s="0"/>
+      <c r="PM9" s="0"/>
+      <c r="PN9" s="0"/>
+      <c r="PO9" s="0"/>
+      <c r="PP9" s="0"/>
+      <c r="PQ9" s="0"/>
+      <c r="PR9" s="0"/>
+      <c r="PS9" s="0"/>
+      <c r="PT9" s="0"/>
+      <c r="PU9" s="0"/>
+      <c r="PV9" s="0"/>
+      <c r="PW9" s="0"/>
+      <c r="PX9" s="0"/>
+      <c r="PY9" s="0"/>
+      <c r="PZ9" s="0"/>
+      <c r="QA9" s="0"/>
+      <c r="QB9" s="0"/>
+      <c r="QC9" s="0"/>
+      <c r="QD9" s="0"/>
+      <c r="QE9" s="0"/>
+      <c r="QF9" s="0"/>
+      <c r="QG9" s="0"/>
+      <c r="QH9" s="0"/>
+      <c r="QI9" s="0"/>
+      <c r="QJ9" s="0"/>
+      <c r="QK9" s="0"/>
+      <c r="QL9" s="0"/>
+      <c r="QM9" s="0"/>
+      <c r="QN9" s="0"/>
+      <c r="QO9" s="0"/>
+      <c r="QP9" s="0"/>
+      <c r="QQ9" s="0"/>
+      <c r="QR9" s="0"/>
+      <c r="QS9" s="0"/>
+      <c r="QT9" s="0"/>
+      <c r="QU9" s="0"/>
+      <c r="QV9" s="0"/>
+      <c r="QW9" s="0"/>
+      <c r="QX9" s="0"/>
+      <c r="QY9" s="0"/>
+      <c r="QZ9" s="0"/>
+      <c r="RA9" s="0"/>
+      <c r="RB9" s="0"/>
+      <c r="RC9" s="0"/>
+      <c r="RD9" s="0"/>
+      <c r="RE9" s="0"/>
+      <c r="RF9" s="0"/>
+      <c r="RG9" s="0"/>
+      <c r="RH9" s="0"/>
+      <c r="RI9" s="0"/>
+      <c r="RJ9" s="0"/>
+      <c r="RK9" s="0"/>
+      <c r="RL9" s="0"/>
+      <c r="RM9" s="0"/>
+      <c r="RN9" s="0"/>
+      <c r="RO9" s="0"/>
+      <c r="RP9" s="0"/>
+      <c r="RQ9" s="0"/>
+      <c r="RR9" s="0"/>
+      <c r="RS9" s="0"/>
+      <c r="RT9" s="0"/>
+      <c r="RU9" s="0"/>
+      <c r="RV9" s="0"/>
+      <c r="RW9" s="0"/>
+      <c r="RX9" s="0"/>
+      <c r="RY9" s="0"/>
+      <c r="RZ9" s="0"/>
+      <c r="SA9" s="0"/>
+      <c r="SB9" s="0"/>
+      <c r="SC9" s="0"/>
+      <c r="SD9" s="0"/>
+      <c r="SE9" s="0"/>
+      <c r="SF9" s="0"/>
+      <c r="SG9" s="0"/>
+      <c r="SH9" s="0"/>
+      <c r="SI9" s="0"/>
+      <c r="SJ9" s="0"/>
+      <c r="SK9" s="0"/>
+      <c r="SL9" s="0"/>
+      <c r="SM9" s="0"/>
+      <c r="SN9" s="0"/>
+      <c r="SO9" s="0"/>
+      <c r="SP9" s="0"/>
+      <c r="SQ9" s="0"/>
+      <c r="SR9" s="0"/>
+      <c r="SS9" s="0"/>
+      <c r="ST9" s="0"/>
+      <c r="SU9" s="0"/>
+      <c r="SV9" s="0"/>
+      <c r="SW9" s="0"/>
+      <c r="SX9" s="0"/>
+      <c r="SY9" s="0"/>
+      <c r="SZ9" s="0"/>
+      <c r="TA9" s="0"/>
+      <c r="TB9" s="0"/>
+      <c r="TC9" s="0"/>
+      <c r="TD9" s="0"/>
+      <c r="TE9" s="0"/>
+      <c r="TF9" s="0"/>
+      <c r="TG9" s="0"/>
+      <c r="TH9" s="0"/>
+      <c r="TI9" s="0"/>
+      <c r="TJ9" s="0"/>
+      <c r="TK9" s="0"/>
+      <c r="TL9" s="0"/>
+      <c r="TM9" s="0"/>
+      <c r="TN9" s="0"/>
+      <c r="TO9" s="0"/>
+      <c r="TP9" s="0"/>
+      <c r="TQ9" s="0"/>
+      <c r="TR9" s="0"/>
+      <c r="TS9" s="0"/>
+      <c r="TT9" s="0"/>
+      <c r="TU9" s="0"/>
+      <c r="TV9" s="0"/>
+      <c r="TW9" s="0"/>
+      <c r="TX9" s="0"/>
+      <c r="TY9" s="0"/>
+      <c r="TZ9" s="0"/>
+      <c r="UA9" s="0"/>
+      <c r="UB9" s="0"/>
+      <c r="UC9" s="0"/>
+      <c r="UD9" s="0"/>
+      <c r="UE9" s="0"/>
+      <c r="UF9" s="0"/>
+      <c r="UG9" s="0"/>
+      <c r="UH9" s="0"/>
+      <c r="UI9" s="0"/>
+      <c r="UJ9" s="0"/>
+      <c r="UK9" s="0"/>
+      <c r="UL9" s="0"/>
+      <c r="UM9" s="0"/>
+      <c r="UN9" s="0"/>
+      <c r="UO9" s="0"/>
+      <c r="UP9" s="0"/>
+      <c r="UQ9" s="0"/>
+      <c r="UR9" s="0"/>
+      <c r="US9" s="0"/>
+      <c r="UT9" s="0"/>
+      <c r="UU9" s="0"/>
+      <c r="UV9" s="0"/>
+      <c r="UW9" s="0"/>
+      <c r="UX9" s="0"/>
+      <c r="UY9" s="0"/>
+      <c r="UZ9" s="0"/>
+      <c r="VA9" s="0"/>
+      <c r="VB9" s="0"/>
+      <c r="VC9" s="0"/>
+      <c r="VD9" s="0"/>
+      <c r="VE9" s="0"/>
+      <c r="VF9" s="0"/>
+      <c r="VG9" s="0"/>
+      <c r="VH9" s="0"/>
+      <c r="VI9" s="0"/>
+      <c r="VJ9" s="0"/>
+      <c r="VK9" s="0"/>
+      <c r="VL9" s="0"/>
+      <c r="VM9" s="0"/>
+      <c r="VN9" s="0"/>
+      <c r="VO9" s="0"/>
+      <c r="VP9" s="0"/>
+      <c r="VQ9" s="0"/>
+      <c r="VR9" s="0"/>
+      <c r="VS9" s="0"/>
+      <c r="VT9" s="0"/>
+      <c r="VU9" s="0"/>
+      <c r="VV9" s="0"/>
+      <c r="VW9" s="0"/>
+      <c r="VX9" s="0"/>
+      <c r="VY9" s="0"/>
+      <c r="VZ9" s="0"/>
+      <c r="WA9" s="0"/>
+      <c r="WB9" s="0"/>
+      <c r="WC9" s="0"/>
+      <c r="WD9" s="0"/>
+      <c r="WE9" s="0"/>
+      <c r="WF9" s="0"/>
+      <c r="WG9" s="0"/>
+      <c r="WH9" s="0"/>
+      <c r="WI9" s="0"/>
+      <c r="WJ9" s="0"/>
+      <c r="WK9" s="0"/>
+      <c r="WL9" s="0"/>
+      <c r="WM9" s="0"/>
+      <c r="WN9" s="0"/>
+      <c r="WO9" s="0"/>
+      <c r="WP9" s="0"/>
+      <c r="WQ9" s="0"/>
+      <c r="WR9" s="0"/>
+      <c r="WS9" s="0"/>
+      <c r="WT9" s="0"/>
+      <c r="WU9" s="0"/>
+      <c r="WV9" s="0"/>
+      <c r="WW9" s="0"/>
+      <c r="WX9" s="0"/>
+      <c r="WY9" s="0"/>
+      <c r="WZ9" s="0"/>
+      <c r="XA9" s="0"/>
+      <c r="XB9" s="0"/>
+      <c r="XC9" s="0"/>
+      <c r="XD9" s="0"/>
+      <c r="XE9" s="0"/>
+      <c r="XF9" s="0"/>
+      <c r="XG9" s="0"/>
+      <c r="XH9" s="0"/>
+      <c r="XI9" s="0"/>
+      <c r="XJ9" s="0"/>
+      <c r="XK9" s="0"/>
+      <c r="XL9" s="0"/>
+      <c r="XM9" s="0"/>
+      <c r="XN9" s="0"/>
+      <c r="XO9" s="0"/>
+      <c r="XP9" s="0"/>
+      <c r="XQ9" s="0"/>
+      <c r="XR9" s="0"/>
+      <c r="XS9" s="0"/>
+      <c r="XT9" s="0"/>
+      <c r="XU9" s="0"/>
+      <c r="XV9" s="0"/>
+      <c r="XW9" s="0"/>
+      <c r="XX9" s="0"/>
+      <c r="XY9" s="0"/>
+      <c r="XZ9" s="0"/>
+      <c r="YA9" s="0"/>
+      <c r="YB9" s="0"/>
+      <c r="YC9" s="0"/>
+      <c r="YD9" s="0"/>
+      <c r="YE9" s="0"/>
+      <c r="YF9" s="0"/>
+      <c r="YG9" s="0"/>
+      <c r="YH9" s="0"/>
+      <c r="YI9" s="0"/>
+      <c r="YJ9" s="0"/>
+      <c r="YK9" s="0"/>
+      <c r="YL9" s="0"/>
+      <c r="YM9" s="0"/>
+      <c r="YN9" s="0"/>
+      <c r="YO9" s="0"/>
+      <c r="YP9" s="0"/>
+      <c r="YQ9" s="0"/>
+      <c r="YR9" s="0"/>
+      <c r="YS9" s="0"/>
+      <c r="YT9" s="0"/>
+      <c r="YU9" s="0"/>
+      <c r="YV9" s="0"/>
+      <c r="YW9" s="0"/>
+      <c r="YX9" s="0"/>
+      <c r="YY9" s="0"/>
+      <c r="YZ9" s="0"/>
+      <c r="ZA9" s="0"/>
+      <c r="ZB9" s="0"/>
+      <c r="ZC9" s="0"/>
+      <c r="ZD9" s="0"/>
+      <c r="ZE9" s="0"/>
+      <c r="ZF9" s="0"/>
+      <c r="ZG9" s="0"/>
+      <c r="ZH9" s="0"/>
+      <c r="ZI9" s="0"/>
+      <c r="ZJ9" s="0"/>
+      <c r="ZK9" s="0"/>
+      <c r="ZL9" s="0"/>
+      <c r="ZM9" s="0"/>
+      <c r="ZN9" s="0"/>
+      <c r="ZO9" s="0"/>
+      <c r="ZP9" s="0"/>
+      <c r="ZQ9" s="0"/>
+      <c r="ZR9" s="0"/>
+      <c r="ZS9" s="0"/>
+      <c r="ZT9" s="0"/>
+      <c r="ZU9" s="0"/>
+      <c r="ZV9" s="0"/>
+      <c r="ZW9" s="0"/>
+      <c r="ZX9" s="0"/>
+      <c r="ZY9" s="0"/>
+      <c r="ZZ9" s="0"/>
+      <c r="AAA9" s="0"/>
+      <c r="AAB9" s="0"/>
+      <c r="AAC9" s="0"/>
+      <c r="AAD9" s="0"/>
+      <c r="AAE9" s="0"/>
+      <c r="AAF9" s="0"/>
+      <c r="AAG9" s="0"/>
+      <c r="AAH9" s="0"/>
+      <c r="AAI9" s="0"/>
+      <c r="AAJ9" s="0"/>
+      <c r="AAK9" s="0"/>
+      <c r="AAL9" s="0"/>
+      <c r="AAM9" s="0"/>
+      <c r="AAN9" s="0"/>
+      <c r="AAO9" s="0"/>
+      <c r="AAP9" s="0"/>
+      <c r="AAQ9" s="0"/>
+      <c r="AAR9" s="0"/>
+      <c r="AAS9" s="0"/>
+      <c r="AAT9" s="0"/>
+      <c r="AAU9" s="0"/>
+      <c r="AAV9" s="0"/>
+      <c r="AAW9" s="0"/>
+      <c r="AAX9" s="0"/>
+      <c r="AAY9" s="0"/>
+      <c r="AAZ9" s="0"/>
+      <c r="ABA9" s="0"/>
+      <c r="ABB9" s="0"/>
+      <c r="ABC9" s="0"/>
+      <c r="ABD9" s="0"/>
+      <c r="ABE9" s="0"/>
+      <c r="ABF9" s="0"/>
+      <c r="ABG9" s="0"/>
+      <c r="ABH9" s="0"/>
+      <c r="ABI9" s="0"/>
+      <c r="ABJ9" s="0"/>
+      <c r="ABK9" s="0"/>
+      <c r="ABL9" s="0"/>
+      <c r="ABM9" s="0"/>
+      <c r="ABN9" s="0"/>
+      <c r="ABO9" s="0"/>
+      <c r="ABP9" s="0"/>
+      <c r="ABQ9" s="0"/>
+      <c r="ABR9" s="0"/>
+      <c r="ABS9" s="0"/>
+      <c r="ABT9" s="0"/>
+      <c r="ABU9" s="0"/>
+      <c r="ABV9" s="0"/>
+      <c r="ABW9" s="0"/>
+      <c r="ABX9" s="0"/>
+      <c r="ABY9" s="0"/>
+      <c r="ABZ9" s="0"/>
+      <c r="ACA9" s="0"/>
+      <c r="ACB9" s="0"/>
+      <c r="ACC9" s="0"/>
+      <c r="ACD9" s="0"/>
+      <c r="ACE9" s="0"/>
+      <c r="ACF9" s="0"/>
+      <c r="ACG9" s="0"/>
+      <c r="ACH9" s="0"/>
+      <c r="ACI9" s="0"/>
+      <c r="ACJ9" s="0"/>
+      <c r="ACK9" s="0"/>
+      <c r="ACL9" s="0"/>
+      <c r="ACM9" s="0"/>
+      <c r="ACN9" s="0"/>
+      <c r="ACO9" s="0"/>
+      <c r="ACP9" s="0"/>
+      <c r="ACQ9" s="0"/>
+      <c r="ACR9" s="0"/>
+      <c r="ACS9" s="0"/>
+      <c r="ACT9" s="0"/>
+      <c r="ACU9" s="0"/>
+      <c r="ACV9" s="0"/>
+      <c r="ACW9" s="0"/>
+      <c r="ACX9" s="0"/>
+      <c r="ACY9" s="0"/>
+      <c r="ACZ9" s="0"/>
+      <c r="ADA9" s="0"/>
+      <c r="ADB9" s="0"/>
+      <c r="ADC9" s="0"/>
+      <c r="ADD9" s="0"/>
+      <c r="ADE9" s="0"/>
+      <c r="ADF9" s="0"/>
+      <c r="ADG9" s="0"/>
+      <c r="ADH9" s="0"/>
+      <c r="ADI9" s="0"/>
+      <c r="ADJ9" s="0"/>
+      <c r="ADK9" s="0"/>
+      <c r="ADL9" s="0"/>
+      <c r="ADM9" s="0"/>
+      <c r="ADN9" s="0"/>
+      <c r="ADO9" s="0"/>
+      <c r="ADP9" s="0"/>
+      <c r="ADQ9" s="0"/>
+      <c r="ADR9" s="0"/>
+      <c r="ADS9" s="0"/>
+      <c r="ADT9" s="0"/>
+      <c r="ADU9" s="0"/>
+      <c r="ADV9" s="0"/>
+      <c r="ADW9" s="0"/>
+      <c r="ADX9" s="0"/>
+      <c r="ADY9" s="0"/>
+      <c r="ADZ9" s="0"/>
+      <c r="AEA9" s="0"/>
+      <c r="AEB9" s="0"/>
+      <c r="AEC9" s="0"/>
+      <c r="AED9" s="0"/>
+      <c r="AEE9" s="0"/>
+      <c r="AEF9" s="0"/>
+      <c r="AEG9" s="0"/>
+      <c r="AEH9" s="0"/>
+      <c r="AEI9" s="0"/>
+      <c r="AEJ9" s="0"/>
+      <c r="AEK9" s="0"/>
+      <c r="AEL9" s="0"/>
+      <c r="AEM9" s="0"/>
+      <c r="AEN9" s="0"/>
+      <c r="AEO9" s="0"/>
+      <c r="AEP9" s="0"/>
+      <c r="AEQ9" s="0"/>
+      <c r="AER9" s="0"/>
+      <c r="AES9" s="0"/>
+      <c r="AET9" s="0"/>
+      <c r="AEU9" s="0"/>
+      <c r="AEV9" s="0"/>
+      <c r="AEW9" s="0"/>
+      <c r="AEX9" s="0"/>
+      <c r="AEY9" s="0"/>
+      <c r="AEZ9" s="0"/>
+      <c r="AFA9" s="0"/>
+      <c r="AFB9" s="0"/>
+      <c r="AFC9" s="0"/>
+      <c r="AFD9" s="0"/>
+      <c r="AFE9" s="0"/>
+      <c r="AFF9" s="0"/>
+      <c r="AFG9" s="0"/>
+      <c r="AFH9" s="0"/>
+      <c r="AFI9" s="0"/>
+      <c r="AFJ9" s="0"/>
+      <c r="AFK9" s="0"/>
+      <c r="AFL9" s="0"/>
+      <c r="AFM9" s="0"/>
+      <c r="AFN9" s="0"/>
+      <c r="AFO9" s="0"/>
+      <c r="AFP9" s="0"/>
+      <c r="AFQ9" s="0"/>
+      <c r="AFR9" s="0"/>
+      <c r="AFS9" s="0"/>
+      <c r="AFT9" s="0"/>
+      <c r="AFU9" s="0"/>
+      <c r="AFV9" s="0"/>
+      <c r="AFW9" s="0"/>
+      <c r="AFX9" s="0"/>
+      <c r="AFY9" s="0"/>
+      <c r="AFZ9" s="0"/>
+      <c r="AGA9" s="0"/>
+      <c r="AGB9" s="0"/>
+      <c r="AGC9" s="0"/>
+      <c r="AGD9" s="0"/>
+      <c r="AGE9" s="0"/>
+      <c r="AGF9" s="0"/>
+      <c r="AGG9" s="0"/>
+      <c r="AGH9" s="0"/>
+      <c r="AGI9" s="0"/>
+      <c r="AGJ9" s="0"/>
+      <c r="AGK9" s="0"/>
+      <c r="AGL9" s="0"/>
+      <c r="AGM9" s="0"/>
+      <c r="AGN9" s="0"/>
+      <c r="AGO9" s="0"/>
+      <c r="AGP9" s="0"/>
+      <c r="AGQ9" s="0"/>
+      <c r="AGR9" s="0"/>
+      <c r="AGS9" s="0"/>
+      <c r="AGT9" s="0"/>
+      <c r="AGU9" s="0"/>
+      <c r="AGV9" s="0"/>
+      <c r="AGW9" s="0"/>
+      <c r="AGX9" s="0"/>
+      <c r="AGY9" s="0"/>
+      <c r="AGZ9" s="0"/>
+      <c r="AHA9" s="0"/>
+      <c r="AHB9" s="0"/>
+      <c r="AHC9" s="0"/>
+      <c r="AHD9" s="0"/>
+      <c r="AHE9" s="0"/>
+      <c r="AHF9" s="0"/>
+      <c r="AHG9" s="0"/>
+      <c r="AHH9" s="0"/>
+      <c r="AHI9" s="0"/>
+      <c r="AHJ9" s="0"/>
+      <c r="AHK9" s="0"/>
+      <c r="AHL9" s="0"/>
+      <c r="AHM9" s="0"/>
+      <c r="AHN9" s="0"/>
+      <c r="AHO9" s="0"/>
+      <c r="AHP9" s="0"/>
+      <c r="AHQ9" s="0"/>
+      <c r="AHR9" s="0"/>
+      <c r="AHS9" s="0"/>
+      <c r="AHT9" s="0"/>
+      <c r="AHU9" s="0"/>
+      <c r="AHV9" s="0"/>
+      <c r="AHW9" s="0"/>
+      <c r="AHX9" s="0"/>
+      <c r="AHY9" s="0"/>
+      <c r="AHZ9" s="0"/>
+      <c r="AIA9" s="0"/>
+      <c r="AIB9" s="0"/>
+      <c r="AIC9" s="0"/>
+      <c r="AID9" s="0"/>
+      <c r="AIE9" s="0"/>
+      <c r="AIF9" s="0"/>
+      <c r="AIG9" s="0"/>
+      <c r="AIH9" s="0"/>
+      <c r="AII9" s="0"/>
+      <c r="AIJ9" s="0"/>
+      <c r="AIK9" s="0"/>
+      <c r="AIL9" s="0"/>
+      <c r="AIM9" s="0"/>
+      <c r="AIN9" s="0"/>
+      <c r="AIO9" s="0"/>
+      <c r="AIP9" s="0"/>
+      <c r="AIQ9" s="0"/>
+      <c r="AIR9" s="0"/>
+      <c r="AIS9" s="0"/>
+      <c r="AIT9" s="0"/>
+      <c r="AIU9" s="0"/>
+      <c r="AIV9" s="0"/>
+      <c r="AIW9" s="0"/>
+      <c r="AIX9" s="0"/>
+      <c r="AIY9" s="0"/>
+      <c r="AIZ9" s="0"/>
+      <c r="AJA9" s="0"/>
+      <c r="AJB9" s="0"/>
+      <c r="AJC9" s="0"/>
+      <c r="AJD9" s="0"/>
+      <c r="AJE9" s="0"/>
+      <c r="AJF9" s="0"/>
+      <c r="AJG9" s="0"/>
+      <c r="AJH9" s="0"/>
+      <c r="AJI9" s="0"/>
+      <c r="AJJ9" s="0"/>
+      <c r="AJK9" s="0"/>
+      <c r="AJL9" s="0"/>
+      <c r="AJM9" s="0"/>
+      <c r="AJN9" s="0"/>
+      <c r="AJO9" s="0"/>
+      <c r="AJP9" s="0"/>
+      <c r="AJQ9" s="0"/>
+      <c r="AJR9" s="0"/>
+      <c r="AJS9" s="0"/>
+      <c r="AJT9" s="0"/>
+      <c r="AJU9" s="0"/>
+      <c r="AJV9" s="0"/>
+      <c r="AJW9" s="0"/>
+      <c r="AJX9" s="0"/>
+      <c r="AJY9" s="0"/>
+      <c r="AJZ9" s="0"/>
+      <c r="AKA9" s="0"/>
+      <c r="AKB9" s="0"/>
+      <c r="AKC9" s="0"/>
+      <c r="AKD9" s="0"/>
+      <c r="AKE9" s="0"/>
+      <c r="AKF9" s="0"/>
+      <c r="AKG9" s="0"/>
+      <c r="AKH9" s="0"/>
+      <c r="AKI9" s="0"/>
+      <c r="AKJ9" s="0"/>
+      <c r="AKK9" s="0"/>
+      <c r="AKL9" s="0"/>
+      <c r="AKM9" s="0"/>
+      <c r="AKN9" s="0"/>
+      <c r="AKO9" s="0"/>
+      <c r="AKP9" s="0"/>
+      <c r="AKQ9" s="0"/>
+      <c r="AKR9" s="0"/>
+      <c r="AKS9" s="0"/>
+      <c r="AKT9" s="0"/>
+      <c r="AKU9" s="0"/>
+      <c r="AKV9" s="0"/>
+      <c r="AKW9" s="0"/>
+      <c r="AKX9" s="0"/>
+      <c r="AKY9" s="0"/>
+      <c r="AKZ9" s="0"/>
+      <c r="ALA9" s="0"/>
+      <c r="ALB9" s="0"/>
+      <c r="ALC9" s="0"/>
+      <c r="ALD9" s="0"/>
+      <c r="ALE9" s="0"/>
+      <c r="ALF9" s="0"/>
+      <c r="ALG9" s="0"/>
+      <c r="ALH9" s="0"/>
+      <c r="ALI9" s="0"/>
+      <c r="ALJ9" s="0"/>
+      <c r="ALK9" s="0"/>
+      <c r="ALL9" s="0"/>
+      <c r="ALM9" s="0"/>
+      <c r="ALN9" s="0"/>
+      <c r="ALO9" s="0"/>
+      <c r="ALP9" s="0"/>
+      <c r="ALQ9" s="0"/>
+      <c r="ALR9" s="0"/>
+      <c r="ALS9" s="0"/>
+      <c r="ALT9" s="0"/>
+      <c r="ALU9" s="0"/>
+      <c r="ALV9" s="0"/>
+      <c r="ALW9" s="0"/>
+      <c r="ALX9" s="0"/>
+      <c r="ALY9" s="0"/>
+      <c r="ALZ9" s="0"/>
+      <c r="AMA9" s="0"/>
+      <c r="AMB9" s="0"/>
+      <c r="AMC9" s="0"/>
+      <c r="AMD9" s="0"/>
+      <c r="AME9" s="0"/>
+      <c r="AMF9" s="0"/>
+      <c r="AMG9" s="0"/>
+      <c r="AMH9" s="0"/>
+      <c r="AMI9" s="0"/>
+      <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" s="24" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="20"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -3278,9 +5305,1023 @@
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
-      <c r="H10" s="22"/>
+      <c r="H10" s="20"/>
       <c r="I10" s="22"/>
-      <c r="J10" s="23"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="0"/>
+      <c r="M10" s="0"/>
+      <c r="N10" s="0"/>
+      <c r="O10" s="0"/>
+      <c r="P10" s="0"/>
+      <c r="Q10" s="0"/>
+      <c r="R10" s="0"/>
+      <c r="S10" s="0"/>
+      <c r="T10" s="0"/>
+      <c r="U10" s="0"/>
+      <c r="V10" s="0"/>
+      <c r="W10" s="0"/>
+      <c r="X10" s="0"/>
+      <c r="Y10" s="0"/>
+      <c r="Z10" s="0"/>
+      <c r="AA10" s="0"/>
+      <c r="AB10" s="0"/>
+      <c r="AC10" s="0"/>
+      <c r="AD10" s="0"/>
+      <c r="AE10" s="0"/>
+      <c r="AF10" s="0"/>
+      <c r="AG10" s="0"/>
+      <c r="AH10" s="0"/>
+      <c r="AI10" s="0"/>
+      <c r="AJ10" s="0"/>
+      <c r="AK10" s="0"/>
+      <c r="AL10" s="0"/>
+      <c r="AM10" s="0"/>
+      <c r="AN10" s="0"/>
+      <c r="AO10" s="0"/>
+      <c r="AP10" s="0"/>
+      <c r="AQ10" s="0"/>
+      <c r="AR10" s="0"/>
+      <c r="AS10" s="0"/>
+      <c r="AT10" s="0"/>
+      <c r="AU10" s="0"/>
+      <c r="AV10" s="0"/>
+      <c r="AW10" s="0"/>
+      <c r="AX10" s="0"/>
+      <c r="AY10" s="0"/>
+      <c r="AZ10" s="0"/>
+      <c r="BA10" s="0"/>
+      <c r="BB10" s="0"/>
+      <c r="BC10" s="0"/>
+      <c r="BD10" s="0"/>
+      <c r="BE10" s="0"/>
+      <c r="BF10" s="0"/>
+      <c r="BG10" s="0"/>
+      <c r="BH10" s="0"/>
+      <c r="BI10" s="0"/>
+      <c r="BJ10" s="0"/>
+      <c r="BK10" s="0"/>
+      <c r="BL10" s="0"/>
+      <c r="BM10" s="0"/>
+      <c r="BN10" s="0"/>
+      <c r="BO10" s="0"/>
+      <c r="BP10" s="0"/>
+      <c r="BQ10" s="0"/>
+      <c r="BR10" s="0"/>
+      <c r="BS10" s="0"/>
+      <c r="BT10" s="0"/>
+      <c r="BU10" s="0"/>
+      <c r="BV10" s="0"/>
+      <c r="BW10" s="0"/>
+      <c r="BX10" s="0"/>
+      <c r="BY10" s="0"/>
+      <c r="BZ10" s="0"/>
+      <c r="CA10" s="0"/>
+      <c r="CB10" s="0"/>
+      <c r="CC10" s="0"/>
+      <c r="CD10" s="0"/>
+      <c r="CE10" s="0"/>
+      <c r="CF10" s="0"/>
+      <c r="CG10" s="0"/>
+      <c r="CH10" s="0"/>
+      <c r="CI10" s="0"/>
+      <c r="CJ10" s="0"/>
+      <c r="CK10" s="0"/>
+      <c r="CL10" s="0"/>
+      <c r="CM10" s="0"/>
+      <c r="CN10" s="0"/>
+      <c r="CO10" s="0"/>
+      <c r="CP10" s="0"/>
+      <c r="CQ10" s="0"/>
+      <c r="CR10" s="0"/>
+      <c r="CS10" s="0"/>
+      <c r="CT10" s="0"/>
+      <c r="CU10" s="0"/>
+      <c r="CV10" s="0"/>
+      <c r="CW10" s="0"/>
+      <c r="CX10" s="0"/>
+      <c r="CY10" s="0"/>
+      <c r="CZ10" s="0"/>
+      <c r="DA10" s="0"/>
+      <c r="DB10" s="0"/>
+      <c r="DC10" s="0"/>
+      <c r="DD10" s="0"/>
+      <c r="DE10" s="0"/>
+      <c r="DF10" s="0"/>
+      <c r="DG10" s="0"/>
+      <c r="DH10" s="0"/>
+      <c r="DI10" s="0"/>
+      <c r="DJ10" s="0"/>
+      <c r="DK10" s="0"/>
+      <c r="DL10" s="0"/>
+      <c r="DM10" s="0"/>
+      <c r="DN10" s="0"/>
+      <c r="DO10" s="0"/>
+      <c r="DP10" s="0"/>
+      <c r="DQ10" s="0"/>
+      <c r="DR10" s="0"/>
+      <c r="DS10" s="0"/>
+      <c r="DT10" s="0"/>
+      <c r="DU10" s="0"/>
+      <c r="DV10" s="0"/>
+      <c r="DW10" s="0"/>
+      <c r="DX10" s="0"/>
+      <c r="DY10" s="0"/>
+      <c r="DZ10" s="0"/>
+      <c r="EA10" s="0"/>
+      <c r="EB10" s="0"/>
+      <c r="EC10" s="0"/>
+      <c r="ED10" s="0"/>
+      <c r="EE10" s="0"/>
+      <c r="EF10" s="0"/>
+      <c r="EG10" s="0"/>
+      <c r="EH10" s="0"/>
+      <c r="EI10" s="0"/>
+      <c r="EJ10" s="0"/>
+      <c r="EK10" s="0"/>
+      <c r="EL10" s="0"/>
+      <c r="EM10" s="0"/>
+      <c r="EN10" s="0"/>
+      <c r="EO10" s="0"/>
+      <c r="EP10" s="0"/>
+      <c r="EQ10" s="0"/>
+      <c r="ER10" s="0"/>
+      <c r="ES10" s="0"/>
+      <c r="ET10" s="0"/>
+      <c r="EU10" s="0"/>
+      <c r="EV10" s="0"/>
+      <c r="EW10" s="0"/>
+      <c r="EX10" s="0"/>
+      <c r="EY10" s="0"/>
+      <c r="EZ10" s="0"/>
+      <c r="FA10" s="0"/>
+      <c r="FB10" s="0"/>
+      <c r="FC10" s="0"/>
+      <c r="FD10" s="0"/>
+      <c r="FE10" s="0"/>
+      <c r="FF10" s="0"/>
+      <c r="FG10" s="0"/>
+      <c r="FH10" s="0"/>
+      <c r="FI10" s="0"/>
+      <c r="FJ10" s="0"/>
+      <c r="FK10" s="0"/>
+      <c r="FL10" s="0"/>
+      <c r="FM10" s="0"/>
+      <c r="FN10" s="0"/>
+      <c r="FO10" s="0"/>
+      <c r="FP10" s="0"/>
+      <c r="FQ10" s="0"/>
+      <c r="FR10" s="0"/>
+      <c r="FS10" s="0"/>
+      <c r="FT10" s="0"/>
+      <c r="FU10" s="0"/>
+      <c r="FV10" s="0"/>
+      <c r="FW10" s="0"/>
+      <c r="FX10" s="0"/>
+      <c r="FY10" s="0"/>
+      <c r="FZ10" s="0"/>
+      <c r="GA10" s="0"/>
+      <c r="GB10" s="0"/>
+      <c r="GC10" s="0"/>
+      <c r="GD10" s="0"/>
+      <c r="GE10" s="0"/>
+      <c r="GF10" s="0"/>
+      <c r="GG10" s="0"/>
+      <c r="GH10" s="0"/>
+      <c r="GI10" s="0"/>
+      <c r="GJ10" s="0"/>
+      <c r="GK10" s="0"/>
+      <c r="GL10" s="0"/>
+      <c r="GM10" s="0"/>
+      <c r="GN10" s="0"/>
+      <c r="GO10" s="0"/>
+      <c r="GP10" s="0"/>
+      <c r="GQ10" s="0"/>
+      <c r="GR10" s="0"/>
+      <c r="GS10" s="0"/>
+      <c r="GT10" s="0"/>
+      <c r="GU10" s="0"/>
+      <c r="GV10" s="0"/>
+      <c r="GW10" s="0"/>
+      <c r="GX10" s="0"/>
+      <c r="GY10" s="0"/>
+      <c r="GZ10" s="0"/>
+      <c r="HA10" s="0"/>
+      <c r="HB10" s="0"/>
+      <c r="HC10" s="0"/>
+      <c r="HD10" s="0"/>
+      <c r="HE10" s="0"/>
+      <c r="HF10" s="0"/>
+      <c r="HG10" s="0"/>
+      <c r="HH10" s="0"/>
+      <c r="HI10" s="0"/>
+      <c r="HJ10" s="0"/>
+      <c r="HK10" s="0"/>
+      <c r="HL10" s="0"/>
+      <c r="HM10" s="0"/>
+      <c r="HN10" s="0"/>
+      <c r="HO10" s="0"/>
+      <c r="HP10" s="0"/>
+      <c r="HQ10" s="0"/>
+      <c r="HR10" s="0"/>
+      <c r="HS10" s="0"/>
+      <c r="HT10" s="0"/>
+      <c r="HU10" s="0"/>
+      <c r="HV10" s="0"/>
+      <c r="HW10" s="0"/>
+      <c r="HX10" s="0"/>
+      <c r="HY10" s="0"/>
+      <c r="HZ10" s="0"/>
+      <c r="IA10" s="0"/>
+      <c r="IB10" s="0"/>
+      <c r="IC10" s="0"/>
+      <c r="ID10" s="0"/>
+      <c r="IE10" s="0"/>
+      <c r="IF10" s="0"/>
+      <c r="IG10" s="0"/>
+      <c r="IH10" s="0"/>
+      <c r="II10" s="0"/>
+      <c r="IJ10" s="0"/>
+      <c r="IK10" s="0"/>
+      <c r="IL10" s="0"/>
+      <c r="IM10" s="0"/>
+      <c r="IN10" s="0"/>
+      <c r="IO10" s="0"/>
+      <c r="IP10" s="0"/>
+      <c r="IQ10" s="0"/>
+      <c r="IR10" s="0"/>
+      <c r="IS10" s="0"/>
+      <c r="IT10" s="0"/>
+      <c r="IU10" s="0"/>
+      <c r="IV10" s="0"/>
+      <c r="IW10" s="0"/>
+      <c r="IX10" s="0"/>
+      <c r="IY10" s="0"/>
+      <c r="IZ10" s="0"/>
+      <c r="JA10" s="0"/>
+      <c r="JB10" s="0"/>
+      <c r="JC10" s="0"/>
+      <c r="JD10" s="0"/>
+      <c r="JE10" s="0"/>
+      <c r="JF10" s="0"/>
+      <c r="JG10" s="0"/>
+      <c r="JH10" s="0"/>
+      <c r="JI10" s="0"/>
+      <c r="JJ10" s="0"/>
+      <c r="JK10" s="0"/>
+      <c r="JL10" s="0"/>
+      <c r="JM10" s="0"/>
+      <c r="JN10" s="0"/>
+      <c r="JO10" s="0"/>
+      <c r="JP10" s="0"/>
+      <c r="JQ10" s="0"/>
+      <c r="JR10" s="0"/>
+      <c r="JS10" s="0"/>
+      <c r="JT10" s="0"/>
+      <c r="JU10" s="0"/>
+      <c r="JV10" s="0"/>
+      <c r="JW10" s="0"/>
+      <c r="JX10" s="0"/>
+      <c r="JY10" s="0"/>
+      <c r="JZ10" s="0"/>
+      <c r="KA10" s="0"/>
+      <c r="KB10" s="0"/>
+      <c r="KC10" s="0"/>
+      <c r="KD10" s="0"/>
+      <c r="KE10" s="0"/>
+      <c r="KF10" s="0"/>
+      <c r="KG10" s="0"/>
+      <c r="KH10" s="0"/>
+      <c r="KI10" s="0"/>
+      <c r="KJ10" s="0"/>
+      <c r="KK10" s="0"/>
+      <c r="KL10" s="0"/>
+      <c r="KM10" s="0"/>
+      <c r="KN10" s="0"/>
+      <c r="KO10" s="0"/>
+      <c r="KP10" s="0"/>
+      <c r="KQ10" s="0"/>
+      <c r="KR10" s="0"/>
+      <c r="KS10" s="0"/>
+      <c r="KT10" s="0"/>
+      <c r="KU10" s="0"/>
+      <c r="KV10" s="0"/>
+      <c r="KW10" s="0"/>
+      <c r="KX10" s="0"/>
+      <c r="KY10" s="0"/>
+      <c r="KZ10" s="0"/>
+      <c r="LA10" s="0"/>
+      <c r="LB10" s="0"/>
+      <c r="LC10" s="0"/>
+      <c r="LD10" s="0"/>
+      <c r="LE10" s="0"/>
+      <c r="LF10" s="0"/>
+      <c r="LG10" s="0"/>
+      <c r="LH10" s="0"/>
+      <c r="LI10" s="0"/>
+      <c r="LJ10" s="0"/>
+      <c r="LK10" s="0"/>
+      <c r="LL10" s="0"/>
+      <c r="LM10" s="0"/>
+      <c r="LN10" s="0"/>
+      <c r="LO10" s="0"/>
+      <c r="LP10" s="0"/>
+      <c r="LQ10" s="0"/>
+      <c r="LR10" s="0"/>
+      <c r="LS10" s="0"/>
+      <c r="LT10" s="0"/>
+      <c r="LU10" s="0"/>
+      <c r="LV10" s="0"/>
+      <c r="LW10" s="0"/>
+      <c r="LX10" s="0"/>
+      <c r="LY10" s="0"/>
+      <c r="LZ10" s="0"/>
+      <c r="MA10" s="0"/>
+      <c r="MB10" s="0"/>
+      <c r="MC10" s="0"/>
+      <c r="MD10" s="0"/>
+      <c r="ME10" s="0"/>
+      <c r="MF10" s="0"/>
+      <c r="MG10" s="0"/>
+      <c r="MH10" s="0"/>
+      <c r="MI10" s="0"/>
+      <c r="MJ10" s="0"/>
+      <c r="MK10" s="0"/>
+      <c r="ML10" s="0"/>
+      <c r="MM10" s="0"/>
+      <c r="MN10" s="0"/>
+      <c r="MO10" s="0"/>
+      <c r="MP10" s="0"/>
+      <c r="MQ10" s="0"/>
+      <c r="MR10" s="0"/>
+      <c r="MS10" s="0"/>
+      <c r="MT10" s="0"/>
+      <c r="MU10" s="0"/>
+      <c r="MV10" s="0"/>
+      <c r="MW10" s="0"/>
+      <c r="MX10" s="0"/>
+      <c r="MY10" s="0"/>
+      <c r="MZ10" s="0"/>
+      <c r="NA10" s="0"/>
+      <c r="NB10" s="0"/>
+      <c r="NC10" s="0"/>
+      <c r="ND10" s="0"/>
+      <c r="NE10" s="0"/>
+      <c r="NF10" s="0"/>
+      <c r="NG10" s="0"/>
+      <c r="NH10" s="0"/>
+      <c r="NI10" s="0"/>
+      <c r="NJ10" s="0"/>
+      <c r="NK10" s="0"/>
+      <c r="NL10" s="0"/>
+      <c r="NM10" s="0"/>
+      <c r="NN10" s="0"/>
+      <c r="NO10" s="0"/>
+      <c r="NP10" s="0"/>
+      <c r="NQ10" s="0"/>
+      <c r="NR10" s="0"/>
+      <c r="NS10" s="0"/>
+      <c r="NT10" s="0"/>
+      <c r="NU10" s="0"/>
+      <c r="NV10" s="0"/>
+      <c r="NW10" s="0"/>
+      <c r="NX10" s="0"/>
+      <c r="NY10" s="0"/>
+      <c r="NZ10" s="0"/>
+      <c r="OA10" s="0"/>
+      <c r="OB10" s="0"/>
+      <c r="OC10" s="0"/>
+      <c r="OD10" s="0"/>
+      <c r="OE10" s="0"/>
+      <c r="OF10" s="0"/>
+      <c r="OG10" s="0"/>
+      <c r="OH10" s="0"/>
+      <c r="OI10" s="0"/>
+      <c r="OJ10" s="0"/>
+      <c r="OK10" s="0"/>
+      <c r="OL10" s="0"/>
+      <c r="OM10" s="0"/>
+      <c r="ON10" s="0"/>
+      <c r="OO10" s="0"/>
+      <c r="OP10" s="0"/>
+      <c r="OQ10" s="0"/>
+      <c r="OR10" s="0"/>
+      <c r="OS10" s="0"/>
+      <c r="OT10" s="0"/>
+      <c r="OU10" s="0"/>
+      <c r="OV10" s="0"/>
+      <c r="OW10" s="0"/>
+      <c r="OX10" s="0"/>
+      <c r="OY10" s="0"/>
+      <c r="OZ10" s="0"/>
+      <c r="PA10" s="0"/>
+      <c r="PB10" s="0"/>
+      <c r="PC10" s="0"/>
+      <c r="PD10" s="0"/>
+      <c r="PE10" s="0"/>
+      <c r="PF10" s="0"/>
+      <c r="PG10" s="0"/>
+      <c r="PH10" s="0"/>
+      <c r="PI10" s="0"/>
+      <c r="PJ10" s="0"/>
+      <c r="PK10" s="0"/>
+      <c r="PL10" s="0"/>
+      <c r="PM10" s="0"/>
+      <c r="PN10" s="0"/>
+      <c r="PO10" s="0"/>
+      <c r="PP10" s="0"/>
+      <c r="PQ10" s="0"/>
+      <c r="PR10" s="0"/>
+      <c r="PS10" s="0"/>
+      <c r="PT10" s="0"/>
+      <c r="PU10" s="0"/>
+      <c r="PV10" s="0"/>
+      <c r="PW10" s="0"/>
+      <c r="PX10" s="0"/>
+      <c r="PY10" s="0"/>
+      <c r="PZ10" s="0"/>
+      <c r="QA10" s="0"/>
+      <c r="QB10" s="0"/>
+      <c r="QC10" s="0"/>
+      <c r="QD10" s="0"/>
+      <c r="QE10" s="0"/>
+      <c r="QF10" s="0"/>
+      <c r="QG10" s="0"/>
+      <c r="QH10" s="0"/>
+      <c r="QI10" s="0"/>
+      <c r="QJ10" s="0"/>
+      <c r="QK10" s="0"/>
+      <c r="QL10" s="0"/>
+      <c r="QM10" s="0"/>
+      <c r="QN10" s="0"/>
+      <c r="QO10" s="0"/>
+      <c r="QP10" s="0"/>
+      <c r="QQ10" s="0"/>
+      <c r="QR10" s="0"/>
+      <c r="QS10" s="0"/>
+      <c r="QT10" s="0"/>
+      <c r="QU10" s="0"/>
+      <c r="QV10" s="0"/>
+      <c r="QW10" s="0"/>
+      <c r="QX10" s="0"/>
+      <c r="QY10" s="0"/>
+      <c r="QZ10" s="0"/>
+      <c r="RA10" s="0"/>
+      <c r="RB10" s="0"/>
+      <c r="RC10" s="0"/>
+      <c r="RD10" s="0"/>
+      <c r="RE10" s="0"/>
+      <c r="RF10" s="0"/>
+      <c r="RG10" s="0"/>
+      <c r="RH10" s="0"/>
+      <c r="RI10" s="0"/>
+      <c r="RJ10" s="0"/>
+      <c r="RK10" s="0"/>
+      <c r="RL10" s="0"/>
+      <c r="RM10" s="0"/>
+      <c r="RN10" s="0"/>
+      <c r="RO10" s="0"/>
+      <c r="RP10" s="0"/>
+      <c r="RQ10" s="0"/>
+      <c r="RR10" s="0"/>
+      <c r="RS10" s="0"/>
+      <c r="RT10" s="0"/>
+      <c r="RU10" s="0"/>
+      <c r="RV10" s="0"/>
+      <c r="RW10" s="0"/>
+      <c r="RX10" s="0"/>
+      <c r="RY10" s="0"/>
+      <c r="RZ10" s="0"/>
+      <c r="SA10" s="0"/>
+      <c r="SB10" s="0"/>
+      <c r="SC10" s="0"/>
+      <c r="SD10" s="0"/>
+      <c r="SE10" s="0"/>
+      <c r="SF10" s="0"/>
+      <c r="SG10" s="0"/>
+      <c r="SH10" s="0"/>
+      <c r="SI10" s="0"/>
+      <c r="SJ10" s="0"/>
+      <c r="SK10" s="0"/>
+      <c r="SL10" s="0"/>
+      <c r="SM10" s="0"/>
+      <c r="SN10" s="0"/>
+      <c r="SO10" s="0"/>
+      <c r="SP10" s="0"/>
+      <c r="SQ10" s="0"/>
+      <c r="SR10" s="0"/>
+      <c r="SS10" s="0"/>
+      <c r="ST10" s="0"/>
+      <c r="SU10" s="0"/>
+      <c r="SV10" s="0"/>
+      <c r="SW10" s="0"/>
+      <c r="SX10" s="0"/>
+      <c r="SY10" s="0"/>
+      <c r="SZ10" s="0"/>
+      <c r="TA10" s="0"/>
+      <c r="TB10" s="0"/>
+      <c r="TC10" s="0"/>
+      <c r="TD10" s="0"/>
+      <c r="TE10" s="0"/>
+      <c r="TF10" s="0"/>
+      <c r="TG10" s="0"/>
+      <c r="TH10" s="0"/>
+      <c r="TI10" s="0"/>
+      <c r="TJ10" s="0"/>
+      <c r="TK10" s="0"/>
+      <c r="TL10" s="0"/>
+      <c r="TM10" s="0"/>
+      <c r="TN10" s="0"/>
+      <c r="TO10" s="0"/>
+      <c r="TP10" s="0"/>
+      <c r="TQ10" s="0"/>
+      <c r="TR10" s="0"/>
+      <c r="TS10" s="0"/>
+      <c r="TT10" s="0"/>
+      <c r="TU10" s="0"/>
+      <c r="TV10" s="0"/>
+      <c r="TW10" s="0"/>
+      <c r="TX10" s="0"/>
+      <c r="TY10" s="0"/>
+      <c r="TZ10" s="0"/>
+      <c r="UA10" s="0"/>
+      <c r="UB10" s="0"/>
+      <c r="UC10" s="0"/>
+      <c r="UD10" s="0"/>
+      <c r="UE10" s="0"/>
+      <c r="UF10" s="0"/>
+      <c r="UG10" s="0"/>
+      <c r="UH10" s="0"/>
+      <c r="UI10" s="0"/>
+      <c r="UJ10" s="0"/>
+      <c r="UK10" s="0"/>
+      <c r="UL10" s="0"/>
+      <c r="UM10" s="0"/>
+      <c r="UN10" s="0"/>
+      <c r="UO10" s="0"/>
+      <c r="UP10" s="0"/>
+      <c r="UQ10" s="0"/>
+      <c r="UR10" s="0"/>
+      <c r="US10" s="0"/>
+      <c r="UT10" s="0"/>
+      <c r="UU10" s="0"/>
+      <c r="UV10" s="0"/>
+      <c r="UW10" s="0"/>
+      <c r="UX10" s="0"/>
+      <c r="UY10" s="0"/>
+      <c r="UZ10" s="0"/>
+      <c r="VA10" s="0"/>
+      <c r="VB10" s="0"/>
+      <c r="VC10" s="0"/>
+      <c r="VD10" s="0"/>
+      <c r="VE10" s="0"/>
+      <c r="VF10" s="0"/>
+      <c r="VG10" s="0"/>
+      <c r="VH10" s="0"/>
+      <c r="VI10" s="0"/>
+      <c r="VJ10" s="0"/>
+      <c r="VK10" s="0"/>
+      <c r="VL10" s="0"/>
+      <c r="VM10" s="0"/>
+      <c r="VN10" s="0"/>
+      <c r="VO10" s="0"/>
+      <c r="VP10" s="0"/>
+      <c r="VQ10" s="0"/>
+      <c r="VR10" s="0"/>
+      <c r="VS10" s="0"/>
+      <c r="VT10" s="0"/>
+      <c r="VU10" s="0"/>
+      <c r="VV10" s="0"/>
+      <c r="VW10" s="0"/>
+      <c r="VX10" s="0"/>
+      <c r="VY10" s="0"/>
+      <c r="VZ10" s="0"/>
+      <c r="WA10" s="0"/>
+      <c r="WB10" s="0"/>
+      <c r="WC10" s="0"/>
+      <c r="WD10" s="0"/>
+      <c r="WE10" s="0"/>
+      <c r="WF10" s="0"/>
+      <c r="WG10" s="0"/>
+      <c r="WH10" s="0"/>
+      <c r="WI10" s="0"/>
+      <c r="WJ10" s="0"/>
+      <c r="WK10" s="0"/>
+      <c r="WL10" s="0"/>
+      <c r="WM10" s="0"/>
+      <c r="WN10" s="0"/>
+      <c r="WO10" s="0"/>
+      <c r="WP10" s="0"/>
+      <c r="WQ10" s="0"/>
+      <c r="WR10" s="0"/>
+      <c r="WS10" s="0"/>
+      <c r="WT10" s="0"/>
+      <c r="WU10" s="0"/>
+      <c r="WV10" s="0"/>
+      <c r="WW10" s="0"/>
+      <c r="WX10" s="0"/>
+      <c r="WY10" s="0"/>
+      <c r="WZ10" s="0"/>
+      <c r="XA10" s="0"/>
+      <c r="XB10" s="0"/>
+      <c r="XC10" s="0"/>
+      <c r="XD10" s="0"/>
+      <c r="XE10" s="0"/>
+      <c r="XF10" s="0"/>
+      <c r="XG10" s="0"/>
+      <c r="XH10" s="0"/>
+      <c r="XI10" s="0"/>
+      <c r="XJ10" s="0"/>
+      <c r="XK10" s="0"/>
+      <c r="XL10" s="0"/>
+      <c r="XM10" s="0"/>
+      <c r="XN10" s="0"/>
+      <c r="XO10" s="0"/>
+      <c r="XP10" s="0"/>
+      <c r="XQ10" s="0"/>
+      <c r="XR10" s="0"/>
+      <c r="XS10" s="0"/>
+      <c r="XT10" s="0"/>
+      <c r="XU10" s="0"/>
+      <c r="XV10" s="0"/>
+      <c r="XW10" s="0"/>
+      <c r="XX10" s="0"/>
+      <c r="XY10" s="0"/>
+      <c r="XZ10" s="0"/>
+      <c r="YA10" s="0"/>
+      <c r="YB10" s="0"/>
+      <c r="YC10" s="0"/>
+      <c r="YD10" s="0"/>
+      <c r="YE10" s="0"/>
+      <c r="YF10" s="0"/>
+      <c r="YG10" s="0"/>
+      <c r="YH10" s="0"/>
+      <c r="YI10" s="0"/>
+      <c r="YJ10" s="0"/>
+      <c r="YK10" s="0"/>
+      <c r="YL10" s="0"/>
+      <c r="YM10" s="0"/>
+      <c r="YN10" s="0"/>
+      <c r="YO10" s="0"/>
+      <c r="YP10" s="0"/>
+      <c r="YQ10" s="0"/>
+      <c r="YR10" s="0"/>
+      <c r="YS10" s="0"/>
+      <c r="YT10" s="0"/>
+      <c r="YU10" s="0"/>
+      <c r="YV10" s="0"/>
+      <c r="YW10" s="0"/>
+      <c r="YX10" s="0"/>
+      <c r="YY10" s="0"/>
+      <c r="YZ10" s="0"/>
+      <c r="ZA10" s="0"/>
+      <c r="ZB10" s="0"/>
+      <c r="ZC10" s="0"/>
+      <c r="ZD10" s="0"/>
+      <c r="ZE10" s="0"/>
+      <c r="ZF10" s="0"/>
+      <c r="ZG10" s="0"/>
+      <c r="ZH10" s="0"/>
+      <c r="ZI10" s="0"/>
+      <c r="ZJ10" s="0"/>
+      <c r="ZK10" s="0"/>
+      <c r="ZL10" s="0"/>
+      <c r="ZM10" s="0"/>
+      <c r="ZN10" s="0"/>
+      <c r="ZO10" s="0"/>
+      <c r="ZP10" s="0"/>
+      <c r="ZQ10" s="0"/>
+      <c r="ZR10" s="0"/>
+      <c r="ZS10" s="0"/>
+      <c r="ZT10" s="0"/>
+      <c r="ZU10" s="0"/>
+      <c r="ZV10" s="0"/>
+      <c r="ZW10" s="0"/>
+      <c r="ZX10" s="0"/>
+      <c r="ZY10" s="0"/>
+      <c r="ZZ10" s="0"/>
+      <c r="AAA10" s="0"/>
+      <c r="AAB10" s="0"/>
+      <c r="AAC10" s="0"/>
+      <c r="AAD10" s="0"/>
+      <c r="AAE10" s="0"/>
+      <c r="AAF10" s="0"/>
+      <c r="AAG10" s="0"/>
+      <c r="AAH10" s="0"/>
+      <c r="AAI10" s="0"/>
+      <c r="AAJ10" s="0"/>
+      <c r="AAK10" s="0"/>
+      <c r="AAL10" s="0"/>
+      <c r="AAM10" s="0"/>
+      <c r="AAN10" s="0"/>
+      <c r="AAO10" s="0"/>
+      <c r="AAP10" s="0"/>
+      <c r="AAQ10" s="0"/>
+      <c r="AAR10" s="0"/>
+      <c r="AAS10" s="0"/>
+      <c r="AAT10" s="0"/>
+      <c r="AAU10" s="0"/>
+      <c r="AAV10" s="0"/>
+      <c r="AAW10" s="0"/>
+      <c r="AAX10" s="0"/>
+      <c r="AAY10" s="0"/>
+      <c r="AAZ10" s="0"/>
+      <c r="ABA10" s="0"/>
+      <c r="ABB10" s="0"/>
+      <c r="ABC10" s="0"/>
+      <c r="ABD10" s="0"/>
+      <c r="ABE10" s="0"/>
+      <c r="ABF10" s="0"/>
+      <c r="ABG10" s="0"/>
+      <c r="ABH10" s="0"/>
+      <c r="ABI10" s="0"/>
+      <c r="ABJ10" s="0"/>
+      <c r="ABK10" s="0"/>
+      <c r="ABL10" s="0"/>
+      <c r="ABM10" s="0"/>
+      <c r="ABN10" s="0"/>
+      <c r="ABO10" s="0"/>
+      <c r="ABP10" s="0"/>
+      <c r="ABQ10" s="0"/>
+      <c r="ABR10" s="0"/>
+      <c r="ABS10" s="0"/>
+      <c r="ABT10" s="0"/>
+      <c r="ABU10" s="0"/>
+      <c r="ABV10" s="0"/>
+      <c r="ABW10" s="0"/>
+      <c r="ABX10" s="0"/>
+      <c r="ABY10" s="0"/>
+      <c r="ABZ10" s="0"/>
+      <c r="ACA10" s="0"/>
+      <c r="ACB10" s="0"/>
+      <c r="ACC10" s="0"/>
+      <c r="ACD10" s="0"/>
+      <c r="ACE10" s="0"/>
+      <c r="ACF10" s="0"/>
+      <c r="ACG10" s="0"/>
+      <c r="ACH10" s="0"/>
+      <c r="ACI10" s="0"/>
+      <c r="ACJ10" s="0"/>
+      <c r="ACK10" s="0"/>
+      <c r="ACL10" s="0"/>
+      <c r="ACM10" s="0"/>
+      <c r="ACN10" s="0"/>
+      <c r="ACO10" s="0"/>
+      <c r="ACP10" s="0"/>
+      <c r="ACQ10" s="0"/>
+      <c r="ACR10" s="0"/>
+      <c r="ACS10" s="0"/>
+      <c r="ACT10" s="0"/>
+      <c r="ACU10" s="0"/>
+      <c r="ACV10" s="0"/>
+      <c r="ACW10" s="0"/>
+      <c r="ACX10" s="0"/>
+      <c r="ACY10" s="0"/>
+      <c r="ACZ10" s="0"/>
+      <c r="ADA10" s="0"/>
+      <c r="ADB10" s="0"/>
+      <c r="ADC10" s="0"/>
+      <c r="ADD10" s="0"/>
+      <c r="ADE10" s="0"/>
+      <c r="ADF10" s="0"/>
+      <c r="ADG10" s="0"/>
+      <c r="ADH10" s="0"/>
+      <c r="ADI10" s="0"/>
+      <c r="ADJ10" s="0"/>
+      <c r="ADK10" s="0"/>
+      <c r="ADL10" s="0"/>
+      <c r="ADM10" s="0"/>
+      <c r="ADN10" s="0"/>
+      <c r="ADO10" s="0"/>
+      <c r="ADP10" s="0"/>
+      <c r="ADQ10" s="0"/>
+      <c r="ADR10" s="0"/>
+      <c r="ADS10" s="0"/>
+      <c r="ADT10" s="0"/>
+      <c r="ADU10" s="0"/>
+      <c r="ADV10" s="0"/>
+      <c r="ADW10" s="0"/>
+      <c r="ADX10" s="0"/>
+      <c r="ADY10" s="0"/>
+      <c r="ADZ10" s="0"/>
+      <c r="AEA10" s="0"/>
+      <c r="AEB10" s="0"/>
+      <c r="AEC10" s="0"/>
+      <c r="AED10" s="0"/>
+      <c r="AEE10" s="0"/>
+      <c r="AEF10" s="0"/>
+      <c r="AEG10" s="0"/>
+      <c r="AEH10" s="0"/>
+      <c r="AEI10" s="0"/>
+      <c r="AEJ10" s="0"/>
+      <c r="AEK10" s="0"/>
+      <c r="AEL10" s="0"/>
+      <c r="AEM10" s="0"/>
+      <c r="AEN10" s="0"/>
+      <c r="AEO10" s="0"/>
+      <c r="AEP10" s="0"/>
+      <c r="AEQ10" s="0"/>
+      <c r="AER10" s="0"/>
+      <c r="AES10" s="0"/>
+      <c r="AET10" s="0"/>
+      <c r="AEU10" s="0"/>
+      <c r="AEV10" s="0"/>
+      <c r="AEW10" s="0"/>
+      <c r="AEX10" s="0"/>
+      <c r="AEY10" s="0"/>
+      <c r="AEZ10" s="0"/>
+      <c r="AFA10" s="0"/>
+      <c r="AFB10" s="0"/>
+      <c r="AFC10" s="0"/>
+      <c r="AFD10" s="0"/>
+      <c r="AFE10" s="0"/>
+      <c r="AFF10" s="0"/>
+      <c r="AFG10" s="0"/>
+      <c r="AFH10" s="0"/>
+      <c r="AFI10" s="0"/>
+      <c r="AFJ10" s="0"/>
+      <c r="AFK10" s="0"/>
+      <c r="AFL10" s="0"/>
+      <c r="AFM10" s="0"/>
+      <c r="AFN10" s="0"/>
+      <c r="AFO10" s="0"/>
+      <c r="AFP10" s="0"/>
+      <c r="AFQ10" s="0"/>
+      <c r="AFR10" s="0"/>
+      <c r="AFS10" s="0"/>
+      <c r="AFT10" s="0"/>
+      <c r="AFU10" s="0"/>
+      <c r="AFV10" s="0"/>
+      <c r="AFW10" s="0"/>
+      <c r="AFX10" s="0"/>
+      <c r="AFY10" s="0"/>
+      <c r="AFZ10" s="0"/>
+      <c r="AGA10" s="0"/>
+      <c r="AGB10" s="0"/>
+      <c r="AGC10" s="0"/>
+      <c r="AGD10" s="0"/>
+      <c r="AGE10" s="0"/>
+      <c r="AGF10" s="0"/>
+      <c r="AGG10" s="0"/>
+      <c r="AGH10" s="0"/>
+      <c r="AGI10" s="0"/>
+      <c r="AGJ10" s="0"/>
+      <c r="AGK10" s="0"/>
+      <c r="AGL10" s="0"/>
+      <c r="AGM10" s="0"/>
+      <c r="AGN10" s="0"/>
+      <c r="AGO10" s="0"/>
+      <c r="AGP10" s="0"/>
+      <c r="AGQ10" s="0"/>
+      <c r="AGR10" s="0"/>
+      <c r="AGS10" s="0"/>
+      <c r="AGT10" s="0"/>
+      <c r="AGU10" s="0"/>
+      <c r="AGV10" s="0"/>
+      <c r="AGW10" s="0"/>
+      <c r="AGX10" s="0"/>
+      <c r="AGY10" s="0"/>
+      <c r="AGZ10" s="0"/>
+      <c r="AHA10" s="0"/>
+      <c r="AHB10" s="0"/>
+      <c r="AHC10" s="0"/>
+      <c r="AHD10" s="0"/>
+      <c r="AHE10" s="0"/>
+      <c r="AHF10" s="0"/>
+      <c r="AHG10" s="0"/>
+      <c r="AHH10" s="0"/>
+      <c r="AHI10" s="0"/>
+      <c r="AHJ10" s="0"/>
+      <c r="AHK10" s="0"/>
+      <c r="AHL10" s="0"/>
+      <c r="AHM10" s="0"/>
+      <c r="AHN10" s="0"/>
+      <c r="AHO10" s="0"/>
+      <c r="AHP10" s="0"/>
+      <c r="AHQ10" s="0"/>
+      <c r="AHR10" s="0"/>
+      <c r="AHS10" s="0"/>
+      <c r="AHT10" s="0"/>
+      <c r="AHU10" s="0"/>
+      <c r="AHV10" s="0"/>
+      <c r="AHW10" s="0"/>
+      <c r="AHX10" s="0"/>
+      <c r="AHY10" s="0"/>
+      <c r="AHZ10" s="0"/>
+      <c r="AIA10" s="0"/>
+      <c r="AIB10" s="0"/>
+      <c r="AIC10" s="0"/>
+      <c r="AID10" s="0"/>
+      <c r="AIE10" s="0"/>
+      <c r="AIF10" s="0"/>
+      <c r="AIG10" s="0"/>
+      <c r="AIH10" s="0"/>
+      <c r="AII10" s="0"/>
+      <c r="AIJ10" s="0"/>
+      <c r="AIK10" s="0"/>
+      <c r="AIL10" s="0"/>
+      <c r="AIM10" s="0"/>
+      <c r="AIN10" s="0"/>
+      <c r="AIO10" s="0"/>
+      <c r="AIP10" s="0"/>
+      <c r="AIQ10" s="0"/>
+      <c r="AIR10" s="0"/>
+      <c r="AIS10" s="0"/>
+      <c r="AIT10" s="0"/>
+      <c r="AIU10" s="0"/>
+      <c r="AIV10" s="0"/>
+      <c r="AIW10" s="0"/>
+      <c r="AIX10" s="0"/>
+      <c r="AIY10" s="0"/>
+      <c r="AIZ10" s="0"/>
+      <c r="AJA10" s="0"/>
+      <c r="AJB10" s="0"/>
+      <c r="AJC10" s="0"/>
+      <c r="AJD10" s="0"/>
+      <c r="AJE10" s="0"/>
+      <c r="AJF10" s="0"/>
+      <c r="AJG10" s="0"/>
+      <c r="AJH10" s="0"/>
+      <c r="AJI10" s="0"/>
+      <c r="AJJ10" s="0"/>
+      <c r="AJK10" s="0"/>
+      <c r="AJL10" s="0"/>
+      <c r="AJM10" s="0"/>
+      <c r="AJN10" s="0"/>
+      <c r="AJO10" s="0"/>
+      <c r="AJP10" s="0"/>
+      <c r="AJQ10" s="0"/>
+      <c r="AJR10" s="0"/>
+      <c r="AJS10" s="0"/>
+      <c r="AJT10" s="0"/>
+      <c r="AJU10" s="0"/>
+      <c r="AJV10" s="0"/>
+      <c r="AJW10" s="0"/>
+      <c r="AJX10" s="0"/>
+      <c r="AJY10" s="0"/>
+      <c r="AJZ10" s="0"/>
+      <c r="AKA10" s="0"/>
+      <c r="AKB10" s="0"/>
+      <c r="AKC10" s="0"/>
+      <c r="AKD10" s="0"/>
+      <c r="AKE10" s="0"/>
+      <c r="AKF10" s="0"/>
+      <c r="AKG10" s="0"/>
+      <c r="AKH10" s="0"/>
+      <c r="AKI10" s="0"/>
+      <c r="AKJ10" s="0"/>
+      <c r="AKK10" s="0"/>
+      <c r="AKL10" s="0"/>
+      <c r="AKM10" s="0"/>
+      <c r="AKN10" s="0"/>
+      <c r="AKO10" s="0"/>
+      <c r="AKP10" s="0"/>
+      <c r="AKQ10" s="0"/>
+      <c r="AKR10" s="0"/>
+      <c r="AKS10" s="0"/>
+      <c r="AKT10" s="0"/>
+      <c r="AKU10" s="0"/>
+      <c r="AKV10" s="0"/>
+      <c r="AKW10" s="0"/>
+      <c r="AKX10" s="0"/>
+      <c r="AKY10" s="0"/>
+      <c r="AKZ10" s="0"/>
+      <c r="ALA10" s="0"/>
+      <c r="ALB10" s="0"/>
+      <c r="ALC10" s="0"/>
+      <c r="ALD10" s="0"/>
+      <c r="ALE10" s="0"/>
+      <c r="ALF10" s="0"/>
+      <c r="ALG10" s="0"/>
+      <c r="ALH10" s="0"/>
+      <c r="ALI10" s="0"/>
+      <c r="ALJ10" s="0"/>
+      <c r="ALK10" s="0"/>
+      <c r="ALL10" s="0"/>
+      <c r="ALM10" s="0"/>
+      <c r="ALN10" s="0"/>
+      <c r="ALO10" s="0"/>
+      <c r="ALP10" s="0"/>
+      <c r="ALQ10" s="0"/>
+      <c r="ALR10" s="0"/>
+      <c r="ALS10" s="0"/>
+      <c r="ALT10" s="0"/>
+      <c r="ALU10" s="0"/>
+      <c r="ALV10" s="0"/>
+      <c r="ALW10" s="0"/>
+      <c r="ALX10" s="0"/>
+      <c r="ALY10" s="0"/>
+      <c r="ALZ10" s="0"/>
+      <c r="AMA10" s="0"/>
+      <c r="AMB10" s="0"/>
+      <c r="AMC10" s="0"/>
+      <c r="AMD10" s="0"/>
+      <c r="AME10" s="0"/>
+      <c r="AMF10" s="0"/>
+      <c r="AMG10" s="0"/>
+      <c r="AMH10" s="0"/>
+      <c r="AMI10" s="0"/>
+      <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="20"/>
@@ -3290,10 +6331,10 @@
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
-      <c r="H11" s="21"/>
+      <c r="H11" s="20"/>
       <c r="I11" s="21"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="0"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="18"/>
       <c r="L11" s="0"/>
       <c r="M11" s="0"/>
       <c r="N11" s="0"/>
@@ -4316,10 +7357,10 @@
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="23"/>
       <c r="J12" s="23"/>
-      <c r="K12" s="0"/>
+      <c r="K12" s="18"/>
       <c r="L12" s="0"/>
       <c r="M12" s="0"/>
       <c r="N12" s="0"/>
@@ -5342,10 +8383,10 @@
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
-      <c r="H13" s="22"/>
+      <c r="H13" s="20"/>
       <c r="I13" s="22"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="0"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="18"/>
       <c r="L13" s="0"/>
       <c r="M13" s="0"/>
       <c r="N13" s="0"/>
@@ -6368,10 +9409,10 @@
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
-      <c r="H14" s="22"/>
+      <c r="H14" s="20"/>
       <c r="I14" s="22"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="0"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="18"/>
       <c r="L14" s="0"/>
       <c r="M14" s="0"/>
       <c r="N14" s="0"/>
@@ -7394,10 +10435,10 @@
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
-      <c r="H15" s="22"/>
+      <c r="H15" s="20"/>
       <c r="I15" s="22"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="0"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="18"/>
       <c r="L15" s="0"/>
       <c r="M15" s="0"/>
       <c r="N15" s="0"/>
@@ -8420,10 +11461,10 @@
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
-      <c r="H16" s="22"/>
+      <c r="H16" s="20"/>
       <c r="I16" s="22"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="0"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="18"/>
       <c r="L16" s="0"/>
       <c r="M16" s="0"/>
       <c r="N16" s="0"/>
@@ -9446,10 +12487,10 @@
       <c r="E17" s="20"/>
       <c r="F17" s="20"/>
       <c r="G17" s="20"/>
-      <c r="H17" s="21"/>
+      <c r="H17" s="20"/>
       <c r="I17" s="21"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="0"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="18"/>
       <c r="L17" s="0"/>
       <c r="M17" s="0"/>
       <c r="N17" s="0"/>
@@ -10472,10 +13513,10 @@
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
-      <c r="H18" s="22"/>
+      <c r="H18" s="20"/>
       <c r="I18" s="22"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="0"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="18"/>
       <c r="L18" s="0"/>
       <c r="M18" s="0"/>
       <c r="N18" s="0"/>
@@ -11498,10 +14539,10 @@
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
-      <c r="H19" s="22"/>
+      <c r="H19" s="20"/>
       <c r="I19" s="22"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="0"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="18"/>
       <c r="L19" s="0"/>
       <c r="M19" s="0"/>
       <c r="N19" s="0"/>
@@ -12524,10 +15565,10 @@
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
-      <c r="H20" s="22"/>
+      <c r="H20" s="20"/>
       <c r="I20" s="22"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="0"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="18"/>
       <c r="L20" s="0"/>
       <c r="M20" s="0"/>
       <c r="N20" s="0"/>
@@ -13550,10 +16591,10 @@
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
-      <c r="H21" s="22"/>
+      <c r="H21" s="20"/>
       <c r="I21" s="22"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="0"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="18"/>
       <c r="L21" s="0"/>
       <c r="M21" s="0"/>
       <c r="N21" s="0"/>
@@ -14568,7 +17609,7 @@
       <c r="AMI21" s="0"/>
       <c r="AMJ21" s="0"/>
     </row>
-    <row r="22" s="27" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" s="25" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="20"/>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -14576,11 +17617,12 @@
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
-      <c r="H22" s="22"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="22"/>
-      <c r="J22" s="26"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="24"/>
     </row>
-    <row r="23" s="27" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" s="25" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="20"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
@@ -14588,11 +17630,12 @@
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
-      <c r="H23" s="22"/>
+      <c r="H23" s="20"/>
       <c r="I23" s="22"/>
-      <c r="J23" s="26"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="24"/>
     </row>
-    <row r="24" s="27" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" s="25" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="20"/>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
@@ -14600,9 +17643,10 @@
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
-      <c r="H24" s="22"/>
+      <c r="H24" s="20"/>
       <c r="I24" s="22"/>
-      <c r="J24" s="26"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="24"/>
     </row>
     <row r="25" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="20"/>
@@ -14612,9 +17656,10 @@
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="26"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="24"/>
     </row>
     <row r="26" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="20"/>
@@ -14624,9 +17669,10 @@
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
-      <c r="H26" s="22"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="22"/>
-      <c r="J26" s="26"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="24"/>
     </row>
     <row r="27" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="20"/>
@@ -14636,9 +17682,10 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
-      <c r="H27" s="22"/>
+      <c r="H27" s="20"/>
       <c r="I27" s="22"/>
-      <c r="J27" s="26"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="24"/>
     </row>
     <row r="28" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="20"/>
@@ -14648,9 +17695,10 @@
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
-      <c r="H28" s="22"/>
+      <c r="H28" s="20"/>
       <c r="I28" s="22"/>
-      <c r="J28" s="26"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="24"/>
     </row>
     <row r="29" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="20"/>
@@ -14660,9 +17708,10 @@
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
-      <c r="H29" s="22"/>
+      <c r="H29" s="20"/>
       <c r="I29" s="22"/>
-      <c r="J29" s="26"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="24"/>
     </row>
     <row r="30" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="20"/>
@@ -14672,9 +17721,10 @@
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
-      <c r="H30" s="21"/>
+      <c r="H30" s="20"/>
       <c r="I30" s="21"/>
-      <c r="J30" s="26"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="24"/>
     </row>
     <row r="31" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="20"/>
@@ -14684,9 +17734,10 @@
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
       <c r="G31" s="20"/>
-      <c r="H31" s="21"/>
+      <c r="H31" s="20"/>
       <c r="I31" s="21"/>
-      <c r="J31" s="26"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="24"/>
     </row>
     <row r="32" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="20"/>
@@ -14696,9 +17747,10 @@
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20"/>
-      <c r="H32" s="21"/>
+      <c r="H32" s="20"/>
       <c r="I32" s="21"/>
-      <c r="J32" s="26"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="24"/>
     </row>
     <row r="33" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="20"/>
@@ -14708,9 +17760,10 @@
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
       <c r="G33" s="20"/>
-      <c r="H33" s="21"/>
+      <c r="H33" s="20"/>
       <c r="I33" s="21"/>
-      <c r="J33" s="26"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="24"/>
     </row>
     <row r="34" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="20"/>
@@ -14720,206 +17773,218 @@
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
       <c r="G34" s="20"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="26"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="24"/>
     </row>
     <row r="35" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="29" t="s">
+      <c r="A35" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="28" t="s">
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28" t="s">
+      <c r="E35" s="14"/>
+      <c r="F35" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I35" s="28" t="s">
+      <c r="G35" s="15"/>
+      <c r="H35" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J35" s="30"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="K35" s="26"/>
     </row>
     <row r="36" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="31"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="30"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="26"/>
     </row>
     <row r="37" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="34"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
     </row>
     <row r="38" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="38" t="s">
-        <v>21</v>
+      <c r="A38" s="34" t="s">
+        <v>22</v>
       </c>
-      <c r="B38" s="38"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="39"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="38" t="s">
-        <v>22</v>
+      <c r="A39" s="34" t="s">
+        <v>23</v>
       </c>
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="35"/>
     </row>
     <row r="40" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="38" t="s">
-        <v>23</v>
+      <c r="A40" s="34" t="s">
+        <v>24</v>
       </c>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="39"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="35"/>
     </row>
     <row r="41" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="39"/>
-    </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="38" t="s">
+      <c r="A41" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="39"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="35"/>
     </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="38" t="s">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="35"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="71">
+  <mergeCells count="73">
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="H2:I3"/>
+    <mergeCell ref="H2:J3"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A4:G4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="I5:J5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="I6:J6"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="I7:J7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="I8:J8"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="I9:J9"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="I10:J10"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="I11:J11"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="I12:J12"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="I13:J13"/>
     <mergeCell ref="C14:D14"/>
-    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="I14:J14"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="I15:J15"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="I16:J16"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="I17:J17"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="I18:J18"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="I19:J19"/>
     <mergeCell ref="C20:D20"/>
-    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="I20:J20"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="I21:J21"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="I22:J22"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="I23:J23"/>
     <mergeCell ref="C24:D24"/>
-    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="I24:J24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="I25:J25"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="I26:J26"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="I27:J27"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="I28:J28"/>
     <mergeCell ref="C29:D29"/>
-    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="I29:J29"/>
     <mergeCell ref="C30:D30"/>
-    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="I30:J30"/>
     <mergeCell ref="C31:D31"/>
-    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="I31:J31"/>
     <mergeCell ref="C32:D32"/>
-    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="I32:J32"/>
     <mergeCell ref="C33:D33"/>
-    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="I33:J33"/>
     <mergeCell ref="C34:D34"/>
-    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="I34:J34"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:I35"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="F36:G36"/>
+    <mergeCell ref="H36:I36"/>
   </mergeCells>
   <conditionalFormatting sqref="B17">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
@@ -14941,48 +18006,43 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B:B">
+  <conditionalFormatting sqref="B8">
     <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8">
+  <conditionalFormatting sqref="B12">
     <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
+  <conditionalFormatting sqref="I12">
     <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12">
+  <conditionalFormatting sqref="B24">
     <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24">
+  <conditionalFormatting sqref="B29:B34">
     <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:B34">
+  <conditionalFormatting sqref="B33">
     <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B33">
+  <conditionalFormatting sqref="B11">
     <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11">
+  <conditionalFormatting sqref="B19">
     <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>